<commit_message>
fixed errors in atmosphere exposure and reran all spp
Former-commit-id: 05ea912e0d6402edd95849a4f191cf2bbc503bf2
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="540" windowWidth="20620" windowHeight="14600" activeTab="2"/>
+    <workbookView xWindow="7720" yWindow="540" windowWidth="20620" windowHeight="14600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sensitivity" sheetId="1" r:id="rId1"/>
@@ -695,13 +695,13 @@
     <t>can't really include those - maybe captured elsewehere</t>
   </si>
   <si>
-    <t>air</t>
-  </si>
-  <si>
     <t>breeding/nesting range/number of spawning aggregations (fish)</t>
   </si>
   <si>
     <t>foraging range</t>
+  </si>
+  <si>
+    <t>atmosphere</t>
   </si>
 </sst>
 </file>
@@ -7568,11 +7568,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8760,7 +8760,7 @@
         <v>108</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D16" s="16">
         <v>1</v>
@@ -9230,7 +9230,7 @@
         <v>115</v>
       </c>
       <c r="D22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="20">
         <v>1</v>
@@ -9652,7 +9652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -10468,7 +10468,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>196</v>
@@ -10482,7 +10482,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>196</v>
@@ -10496,7 +10496,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>196</v>
@@ -10510,7 +10510,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>196</v>
@@ -10524,7 +10524,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>196</v>
@@ -10538,7 +10538,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>201</v>
@@ -10552,7 +10552,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>201</v>
@@ -10566,7 +10566,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B60" s="31" t="s">
         <v>202</v>
@@ -10580,7 +10580,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B61" s="31" t="s">
         <v>202</v>
@@ -10594,7 +10594,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B62" s="31" t="s">
         <v>202</v>
@@ -10608,7 +10608,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B63" s="31" t="s">
         <v>202</v>
@@ -10622,7 +10622,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B64" s="31" t="s">
         <v>201</v>
@@ -10636,7 +10636,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B65" s="31" t="s">
         <v>201</v>

</xml_diff>

<commit_message>
reran all species, after fixing: * photosynthesis (from light dependence) rescored for traits and for species * a bug in air temp (added "atmosphere" to valid trait values) * rescaled vulnerability so scores span 0-1
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="0" windowWidth="20620" windowHeight="14600"/>
+    <workbookView xWindow="1360" yWindow="420" windowWidth="27280" windowHeight="17120"/>
   </bookViews>
   <sheets>
     <sheet name="sensitivity" sheetId="1" r:id="rId1"/>
@@ -939,11 +939,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1235,7 +1235,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1246,11 +1246,11 @@
   <dimension ref="A1:AC86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D47" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
+      <selection pane="bottomRight" activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1263,7 +1263,7 @@
     <col min="10" max="10" width="8.83203125" style="40"/>
     <col min="12" max="12" width="12.33203125" style="19" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" style="19" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="40"/>
+    <col min="16" max="16" width="17.33203125" style="40" customWidth="1"/>
     <col min="20" max="20" width="8.83203125" style="40"/>
     <col min="21" max="21" width="12.33203125" style="19" customWidth="1"/>
     <col min="27" max="27" width="8.83203125" style="36"/>
@@ -7568,11 +7568,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updated species_trait_all and stressor_traits_scored based on convo between Nat and Casey, incl sex ratio and some nudges to have scores better match expert feedback
Former-commit-id: 44a6fc6c3f6e511010ffd15bdf72f093e3cedc45
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Dropbox\Fiji_workshop_after\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C567A5D-A73E-4D89-94DF-B4C939EF4BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8680C81-3BED-4B29-9BC3-4F1DF0B675E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="240" windowWidth="25455" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="1380" windowWidth="22755" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensitivity" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="220">
   <si>
     <t>category</t>
   </si>
@@ -709,6 +709,15 @@
   <si>
     <t>plastic pollution (microplastic)</t>
   </si>
+  <si>
+    <t>Reproduction</t>
+  </si>
+  <si>
+    <t>can the sex ratio be affected by temperature?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no </t>
+  </si>
 </sst>
 </file>
 
@@ -775,7 +784,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -872,6 +881,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -888,7 +903,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -974,6 +989,11 @@
     <xf numFmtId="49" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -983,6 +1003,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1302,11 +1328,11 @@
   <dimension ref="A1:AC3729"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H23" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1:O1048576"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3706,8 +3732,8 @@
       <c r="V31" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="W31" s="56" t="s">
-        <v>137</v>
+      <c r="W31" s="65" t="s">
+        <v>51</v>
       </c>
       <c r="X31" s="57" t="s">
         <v>75</v>
@@ -3783,8 +3809,8 @@
       <c r="V32" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="W32" s="56" t="s">
-        <v>137</v>
+      <c r="W32" s="65" t="s">
+        <v>51</v>
       </c>
       <c r="X32" s="57" t="s">
         <v>137</v>
@@ -3946,8 +3972,8 @@
       <c r="K36" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="L36" s="19" t="s">
-        <v>5</v>
+      <c r="L36" s="65" t="s">
+        <v>75</v>
       </c>
       <c r="M36" s="36" t="s">
         <v>51</v>
@@ -6979,8 +7005,8 @@
       <c r="U75" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="V75" s="36" t="s">
-        <v>75</v>
+      <c r="V75" s="65" t="s">
+        <v>51</v>
       </c>
       <c r="W75" s="36" t="s">
         <v>51</v>
@@ -7056,8 +7082,8 @@
       <c r="U76" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="V76" s="36" t="s">
-        <v>137</v>
+      <c r="V76" s="65" t="s">
+        <v>51</v>
       </c>
       <c r="W76" s="36" t="s">
         <v>51</v>
@@ -7210,8 +7236,8 @@
       <c r="U78" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="V78" s="40" t="s">
-        <v>75</v>
+      <c r="V78" s="65" t="s">
+        <v>51</v>
       </c>
       <c r="W78" s="40" t="s">
         <v>51</v>
@@ -19848,13 +19874,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AB34"/>
+  <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2:O4"/>
+      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20245,7 +20271,7 @@
       <c r="V5" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="W5" s="36" t="s">
+      <c r="W5" s="53" t="s">
         <v>74</v>
       </c>
       <c r="X5" s="36" t="s">
@@ -21036,162 +21062,163 @@
       </c>
       <c r="AB15" s="50"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D16" s="16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="16">
-        <v>0</v>
-      </c>
-      <c r="H16" s="16">
-        <v>0</v>
-      </c>
-      <c r="I16" s="16">
-        <v>1</v>
-      </c>
-      <c r="J16" s="16">
-        <v>0</v>
-      </c>
-      <c r="K16" s="16">
-        <v>1</v>
-      </c>
-      <c r="L16" s="16">
-        <v>1</v>
-      </c>
-      <c r="M16" s="16">
-        <v>0</v>
-      </c>
-      <c r="N16" s="16">
-        <v>0</v>
-      </c>
-      <c r="O16" s="16">
-        <v>0</v>
-      </c>
-      <c r="P16" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="16">
-        <v>0</v>
-      </c>
-      <c r="R16" s="16">
-        <v>0</v>
-      </c>
-      <c r="S16" s="16">
-        <v>0</v>
-      </c>
-      <c r="T16" s="16">
-        <v>0</v>
-      </c>
-      <c r="U16" s="16">
-        <v>1</v>
-      </c>
-      <c r="V16" s="16">
-        <v>1</v>
-      </c>
-      <c r="W16" s="16">
-        <v>1</v>
-      </c>
-      <c r="X16" s="16">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="20">
-        <v>0</v>
-      </c>
-      <c r="E17" s="20">
-        <v>1</v>
-      </c>
-      <c r="F17" s="20">
-        <v>1</v>
-      </c>
-      <c r="G17" s="20">
-        <v>1</v>
-      </c>
-      <c r="H17" s="20">
-        <v>1</v>
-      </c>
-      <c r="I17" s="16">
-        <v>1</v>
-      </c>
-      <c r="J17" s="44">
-        <v>1</v>
-      </c>
-      <c r="K17" s="20">
-        <v>1</v>
-      </c>
-      <c r="L17" s="20">
-        <v>1</v>
-      </c>
-      <c r="M17" s="16">
-        <v>1</v>
-      </c>
-      <c r="N17" s="20">
-        <v>1</v>
-      </c>
-      <c r="O17" s="16">
-        <v>1</v>
-      </c>
-      <c r="P17" s="44">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="16">
-        <v>1</v>
-      </c>
-      <c r="R17" s="20">
-        <v>1</v>
-      </c>
-      <c r="S17" s="20">
-        <v>1</v>
-      </c>
-      <c r="T17" s="20">
-        <v>1</v>
-      </c>
-      <c r="U17" s="20">
-        <v>0</v>
-      </c>
-      <c r="V17" s="16">
-        <v>1</v>
-      </c>
-      <c r="W17" s="16">
-        <v>1</v>
-      </c>
-      <c r="X17" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="16">
-        <v>1</v>
-      </c>
-      <c r="AB17" s="14"/>
-    </row>
-    <row r="18" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="67" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="67" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="M16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="N16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="O16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="R16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="S16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="T16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="U16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="V16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="W16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="X16" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y16" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB16" s="50"/>
+    </row>
+    <row r="17" spans="1:28" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="67" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" s="67" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" s="67" t="s">
+        <v>219</v>
+      </c>
+      <c r="D17" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="L17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="N17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="P17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="R17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="S17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="T17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="U17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="V17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="W17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="X17" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y17" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB17" s="50"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>106</v>
       </c>
@@ -21199,75 +21226,74 @@
         <v>107</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" s="20">
+        <v>210</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
         <v>0</v>
       </c>
-      <c r="E18" s="20">
+      <c r="F18" s="16">
         <v>1</v>
       </c>
-      <c r="F18" s="20">
-        <v>1</v>
-      </c>
-      <c r="G18" s="20">
-        <v>1</v>
-      </c>
-      <c r="H18" s="20">
+      <c r="G18" s="16">
+        <v>0</v>
+      </c>
+      <c r="H18" s="16">
         <v>0</v>
       </c>
       <c r="I18" s="16">
         <v>1</v>
       </c>
-      <c r="J18" s="44">
+      <c r="J18" s="16">
         <v>0</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K18" s="16">
         <v>1</v>
       </c>
-      <c r="L18" s="20">
+      <c r="L18" s="16">
+        <v>1</v>
+      </c>
+      <c r="M18" s="16">
         <v>0</v>
       </c>
-      <c r="M18" s="16">
+      <c r="N18" s="16">
+        <v>0</v>
+      </c>
+      <c r="O18" s="16">
+        <v>0</v>
+      </c>
+      <c r="P18" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="16">
+        <v>0</v>
+      </c>
+      <c r="R18" s="16">
+        <v>0</v>
+      </c>
+      <c r="S18" s="16">
+        <v>0</v>
+      </c>
+      <c r="T18" s="16">
+        <v>0</v>
+      </c>
+      <c r="U18" s="16">
         <v>1</v>
       </c>
-      <c r="N18" s="20">
+      <c r="V18" s="16">
         <v>1</v>
       </c>
-      <c r="O18" s="16">
+      <c r="W18" s="16">
         <v>1</v>
       </c>
-      <c r="P18" s="44">
+      <c r="X18" s="16">
         <v>0</v>
       </c>
-      <c r="Q18" s="16">
+      <c r="Y18" s="16">
         <v>1</v>
       </c>
-      <c r="R18" s="20">
-        <v>0</v>
-      </c>
-      <c r="S18" s="20">
-        <v>1</v>
-      </c>
-      <c r="T18" s="20">
-        <v>0</v>
-      </c>
-      <c r="U18" s="20">
-        <v>0</v>
-      </c>
-      <c r="V18" s="16">
-        <v>0</v>
-      </c>
-      <c r="W18" s="16">
-        <v>0</v>
-      </c>
-      <c r="X18" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="14"/>
     </row>
     <row r="19" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -21277,7 +21303,7 @@
         <v>107</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D19" s="20">
         <v>0</v>
@@ -21289,22 +21315,22 @@
         <v>1</v>
       </c>
       <c r="G19" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="16">
         <v>1</v>
       </c>
       <c r="J19" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="20">
         <v>1</v>
       </c>
       <c r="L19" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="16">
         <v>1</v>
@@ -21316,34 +21342,34 @@
         <v>1</v>
       </c>
       <c r="P19" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="16">
         <v>1</v>
       </c>
       <c r="R19" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19" s="20">
         <v>0</v>
       </c>
       <c r="V19" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W19" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB19" s="14"/>
     </row>
@@ -21355,25 +21381,25 @@
         <v>107</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D20" s="20">
         <v>0</v>
       </c>
       <c r="E20" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="20">
         <v>1</v>
       </c>
       <c r="G20" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="20">
         <v>0</v>
       </c>
-      <c r="I20" s="20">
-        <v>0</v>
+      <c r="I20" s="16">
+        <v>1</v>
       </c>
       <c r="J20" s="44">
         <v>0</v>
@@ -21391,7 +21417,7 @@
         <v>1</v>
       </c>
       <c r="O20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20" s="44">
         <v>0</v>
@@ -21403,7 +21429,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20" s="20">
         <v>0</v>
@@ -21418,12 +21444,12 @@
         <v>0</v>
       </c>
       <c r="X20" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y20" s="16">
         <v>0</v>
       </c>
-      <c r="AB20" s="13"/>
+      <c r="AB20" s="14"/>
     </row>
     <row r="21" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -21433,16 +21459,16 @@
         <v>107</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D21" s="20">
         <v>0</v>
       </c>
       <c r="E21" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="20">
         <v>0</v>
@@ -21451,13 +21477,13 @@
         <v>0</v>
       </c>
       <c r="I21" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="44">
         <v>0</v>
       </c>
       <c r="K21" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" s="20">
         <v>0</v>
@@ -21469,7 +21495,7 @@
         <v>1</v>
       </c>
       <c r="O21" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" s="44">
         <v>0</v>
@@ -21501,44 +21527,44 @@
       <c r="Y21" s="16">
         <v>0</v>
       </c>
-      <c r="AB21" s="15"/>
+      <c r="AB21" s="14"/>
     </row>
     <row r="22" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>114</v>
+      <c r="B22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="D22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="20">
         <v>1</v>
       </c>
       <c r="G22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="20">
-        <v>1</v>
-      </c>
-      <c r="I22" s="16">
         <v>0</v>
       </c>
+      <c r="I22" s="20">
+        <v>0</v>
+      </c>
       <c r="J22" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="20">
         <v>1</v>
       </c>
       <c r="L22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="16">
         <v>1</v>
@@ -21547,75 +21573,76 @@
         <v>1</v>
       </c>
       <c r="O22" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P22" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="16">
         <v>1</v>
       </c>
       <c r="R22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W22" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X22" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y22" s="59">
         <v>0</v>
       </c>
+      <c r="Y22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="13"/>
     </row>
     <row r="23" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>115</v>
+      <c r="B23" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="D23" s="20">
         <v>0</v>
       </c>
       <c r="E23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" s="16">
         <v>1</v>
@@ -21624,38 +21651,39 @@
         <v>1</v>
       </c>
       <c r="O23" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="16">
         <v>1</v>
       </c>
       <c r="R23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V23" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W23" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X23" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y23" s="16">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="15"/>
     </row>
     <row r="24" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -21665,10 +21693,10 @@
         <v>113</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D24" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="20">
         <v>1</v>
@@ -21683,13 +21711,13 @@
         <v>1</v>
       </c>
       <c r="I24" s="16">
+        <v>0</v>
+      </c>
+      <c r="J24" s="44">
         <v>1</v>
       </c>
-      <c r="J24" s="44">
-        <v>0</v>
-      </c>
       <c r="K24" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="20">
         <v>1</v>
@@ -21700,26 +21728,26 @@
       <c r="N24" s="20">
         <v>1</v>
       </c>
-      <c r="O24" s="16">
+      <c r="O24" s="66">
+        <v>0</v>
+      </c>
+      <c r="P24" s="44">
         <v>1</v>
-      </c>
-      <c r="P24" s="44">
-        <v>0</v>
       </c>
       <c r="Q24" s="16">
         <v>1</v>
       </c>
       <c r="R24" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U24" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24" s="16">
         <v>1</v>
@@ -21730,8 +21758,8 @@
       <c r="X24" s="20">
         <v>1</v>
       </c>
-      <c r="Y24" s="16">
-        <v>1</v>
+      <c r="Y24" s="59">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -21742,7 +21770,7 @@
         <v>113</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D25" s="20">
         <v>0</v>
@@ -21777,8 +21805,8 @@
       <c r="N25" s="20">
         <v>1</v>
       </c>
-      <c r="O25" s="16">
-        <v>1</v>
+      <c r="O25" s="66">
+        <v>0</v>
       </c>
       <c r="P25" s="44">
         <v>1</v>
@@ -21796,19 +21824,19 @@
         <v>1</v>
       </c>
       <c r="U25" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V25" s="16">
         <v>1</v>
       </c>
       <c r="W25" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X25" s="20">
         <v>1</v>
       </c>
       <c r="Y25" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
@@ -21819,7 +21847,7 @@
         <v>113</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D26" s="20">
         <v>0</v>
@@ -21840,10 +21868,10 @@
         <v>1</v>
       </c>
       <c r="J26" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" s="20">
         <v>1</v>
@@ -21858,19 +21886,19 @@
         <v>1</v>
       </c>
       <c r="P26" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="16">
         <v>1</v>
       </c>
       <c r="R26" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S26" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T26" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U26" s="20">
         <v>0</v>
@@ -21879,49 +21907,203 @@
         <v>1</v>
       </c>
       <c r="W26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X26" s="20">
         <v>1</v>
       </c>
       <c r="Y26" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="Q27" s="36"/>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="46" t="s">
-        <v>206</v>
-      </c>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="Q28" s="36"/>
+      <c r="E27" s="20">
+        <v>1</v>
+      </c>
+      <c r="F27" s="20">
+        <v>1</v>
+      </c>
+      <c r="G27" s="20">
+        <v>1</v>
+      </c>
+      <c r="H27" s="20">
+        <v>1</v>
+      </c>
+      <c r="I27" s="16">
+        <v>1</v>
+      </c>
+      <c r="J27" s="44">
+        <v>1</v>
+      </c>
+      <c r="K27" s="20">
+        <v>1</v>
+      </c>
+      <c r="L27" s="20">
+        <v>1</v>
+      </c>
+      <c r="M27" s="16">
+        <v>1</v>
+      </c>
+      <c r="N27" s="20">
+        <v>1</v>
+      </c>
+      <c r="O27" s="16">
+        <v>1</v>
+      </c>
+      <c r="P27" s="44">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="16">
+        <v>1</v>
+      </c>
+      <c r="R27" s="20">
+        <v>1</v>
+      </c>
+      <c r="S27" s="20">
+        <v>1</v>
+      </c>
+      <c r="T27" s="20">
+        <v>1</v>
+      </c>
+      <c r="U27" s="20">
+        <v>0</v>
+      </c>
+      <c r="V27" s="16">
+        <v>1</v>
+      </c>
+      <c r="W27" s="16">
+        <v>0</v>
+      </c>
+      <c r="X27" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="20">
+        <v>0</v>
+      </c>
+      <c r="E28" s="20">
+        <v>1</v>
+      </c>
+      <c r="F28" s="20">
+        <v>1</v>
+      </c>
+      <c r="G28" s="20">
+        <v>1</v>
+      </c>
+      <c r="H28" s="20">
+        <v>1</v>
+      </c>
+      <c r="I28" s="16">
+        <v>1</v>
+      </c>
+      <c r="J28" s="44">
+        <v>1</v>
+      </c>
+      <c r="K28" s="20">
+        <v>1</v>
+      </c>
+      <c r="L28" s="20">
+        <v>1</v>
+      </c>
+      <c r="M28" s="16">
+        <v>1</v>
+      </c>
+      <c r="N28" s="20">
+        <v>1</v>
+      </c>
+      <c r="O28" s="66">
+        <v>0</v>
+      </c>
+      <c r="P28" s="44">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="16">
+        <v>1</v>
+      </c>
+      <c r="R28" s="20">
+        <v>1</v>
+      </c>
+      <c r="S28" s="20">
+        <v>1</v>
+      </c>
+      <c r="T28" s="20">
+        <v>1</v>
+      </c>
+      <c r="U28" s="20">
+        <v>0</v>
+      </c>
+      <c r="V28" s="16">
+        <v>1</v>
+      </c>
+      <c r="W28" s="16">
+        <v>0</v>
+      </c>
+      <c r="X28" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Q29" s="36"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="Q30" s="36"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A32" s="46" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="36"/>
     </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="36"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="36"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AB1:AB20">
-    <sortCondition ref="AB1:AB20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AB1:AB22">
+    <sortCondition ref="AB1:AB22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
also, not larva -> no larva ARGH
Former-commit-id: 6b61573bf2fbc3969a44edffc811de9c72c6508e
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="220" windowWidth="24280" windowHeight="15060"/>
+    <workbookView xWindow="840" yWindow="160" windowWidth="24280" windowHeight="15060"/>
   </bookViews>
   <sheets>
     <sheet name="sensitivity" sheetId="1" r:id="rId1"/>
@@ -306,9 +306,6 @@
   </si>
   <si>
     <t>holoplankton</t>
-  </si>
-  <si>
-    <t>not larva</t>
   </si>
   <si>
     <t>Movement</t>
@@ -712,6 +709,9 @@
   <si>
     <t>non-feeding - non-calcifier</t>
   </si>
+  <si>
+    <t>no larva</t>
+  </si>
 </sst>
 </file>
 
@@ -1015,11 +1015,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1311,7 +1311,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1326,7 +1326,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1358,67 +1358,67 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F1" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>128</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>129</v>
       </c>
       <c r="R1" s="15" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T1" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z1" s="29"/>
       <c r="AB1" s="14"/>
@@ -1431,7 +1431,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>5</v>
@@ -1443,7 +1443,7 @@
         <v>51</v>
       </c>
       <c r="G2" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H2" s="36" t="s">
         <v>5</v>
@@ -1455,7 +1455,7 @@
         <v>51</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L2" s="36" t="s">
         <v>51</v>
@@ -1476,7 +1476,7 @@
         <v>74</v>
       </c>
       <c r="R2" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S2" s="43" t="s">
         <v>74</v>
@@ -1485,7 +1485,7 @@
         <v>51</v>
       </c>
       <c r="U2" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V2" t="s">
         <v>75</v>
@@ -1505,7 +1505,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>5</v>
@@ -1517,7 +1517,7 @@
         <v>51</v>
       </c>
       <c r="G3" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H3" s="36" t="s">
         <v>5</v>
@@ -1529,13 +1529,13 @@
         <v>51</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L3" s="36" t="s">
         <v>51</v>
       </c>
       <c r="M3" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N3" s="36" t="s">
         <v>74</v>
@@ -1550,7 +1550,7 @@
         <v>74</v>
       </c>
       <c r="R3" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S3" s="43" t="s">
         <v>74</v>
@@ -1559,7 +1559,7 @@
         <v>51</v>
       </c>
       <c r="U3" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V3" s="36" t="s">
         <v>75</v>
@@ -1579,7 +1579,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>5</v>
@@ -1603,7 +1603,7 @@
         <v>51</v>
       </c>
       <c r="K4" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L4" s="36" t="s">
         <v>51</v>
@@ -1612,7 +1612,7 @@
         <v>74</v>
       </c>
       <c r="N4" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O4" s="27" t="s">
         <v>74</v>
@@ -1624,7 +1624,7 @@
         <v>74</v>
       </c>
       <c r="R4" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S4" s="43" t="s">
         <v>74</v>
@@ -1633,7 +1633,7 @@
         <v>51</v>
       </c>
       <c r="U4" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V4" s="36" t="s">
         <v>75</v>
@@ -1653,7 +1653,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D5" s="36" t="s">
         <v>5</v>
@@ -1677,16 +1677,16 @@
         <v>51</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L5" s="36" t="s">
         <v>51</v>
       </c>
       <c r="M5" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N5" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O5" s="27" t="s">
         <v>74</v>
@@ -1698,7 +1698,7 @@
         <v>74</v>
       </c>
       <c r="R5" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S5" s="27" t="s">
         <v>75</v>
@@ -1707,7 +1707,7 @@
         <v>51</v>
       </c>
       <c r="U5" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V5" s="36" t="s">
         <v>75</v>
@@ -1727,7 +1727,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>85</v>
+        <v>219</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>5</v>
@@ -1763,7 +1763,7 @@
         <v>51</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P6" s="40" t="s">
         <v>51</v>
@@ -1893,7 +1893,7 @@
         <v>5</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>51</v>
@@ -1911,7 +1911,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P8" s="40" t="s">
         <v>5</v>
@@ -1967,7 +1967,7 @@
         <v>5</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>51</v>
@@ -1985,7 +1985,7 @@
         <v>5</v>
       </c>
       <c r="O9" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P9" s="40" t="s">
         <v>5</v>
@@ -2174,7 +2174,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E12" s="40" t="s">
         <v>51</v>
@@ -2231,7 +2231,7 @@
         <v>51</v>
       </c>
       <c r="W12" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X12" s="37" t="s">
         <v>51</v>
@@ -2248,7 +2248,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E13" s="40" t="s">
         <v>51</v>
@@ -2305,7 +2305,7 @@
         <v>51</v>
       </c>
       <c r="W13" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X13" s="37" t="s">
         <v>51</v>
@@ -2500,7 +2500,7 @@
         <v>5</v>
       </c>
       <c r="N16" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O16" s="27" t="s">
         <v>51</v>
@@ -2521,7 +2521,7 @@
         <v>74</v>
       </c>
       <c r="U16" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V16" s="40" t="s">
         <v>51</v>
@@ -2719,7 +2719,7 @@
         <v>51</v>
       </c>
       <c r="M19" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N19" s="27" t="s">
         <v>51</v>
@@ -2944,7 +2944,7 @@
         <v>5</v>
       </c>
       <c r="N22" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O22" s="27" t="s">
         <v>74</v>
@@ -2971,7 +2971,7 @@
         <v>51</v>
       </c>
       <c r="W22" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X22" s="37" t="s">
         <v>51</v>
@@ -3021,7 +3021,7 @@
         <v>51</v>
       </c>
       <c r="O23" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P23" s="40" t="s">
         <v>5</v>
@@ -3033,7 +3033,7 @@
         <v>51</v>
       </c>
       <c r="S23" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T23" s="19" t="s">
         <v>51</v>
@@ -3077,7 +3077,7 @@
         <v>5</v>
       </c>
       <c r="I24" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J24" s="36" t="s">
         <v>51</v>
@@ -3095,13 +3095,13 @@
         <v>51</v>
       </c>
       <c r="O24" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P24" s="40" t="s">
         <v>5</v>
       </c>
       <c r="Q24" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R24" s="36" t="s">
         <v>51</v>
@@ -3299,7 +3299,7 @@
         <v>5</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J27" s="36" t="s">
         <v>51</v>
@@ -3426,7 +3426,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>15</v>
@@ -3483,7 +3483,7 @@
         <v>74</v>
       </c>
       <c r="U29" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V29" s="40" t="s">
         <v>75</v>
@@ -3500,7 +3500,7 @@
         <v>32</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>16</v>
@@ -3586,7 +3586,7 @@
         <v>74</v>
       </c>
       <c r="F31" s="62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G31" s="40" t="s">
         <v>74</v>
@@ -3654,13 +3654,13 @@
         <v>15</v>
       </c>
       <c r="D32" s="57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E32" s="61" t="s">
         <v>74</v>
       </c>
       <c r="F32" s="62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G32" s="40" t="s">
         <v>51</v>
@@ -3705,13 +3705,13 @@
         <v>74</v>
       </c>
       <c r="U32" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V32" s="65" t="s">
         <v>51</v>
       </c>
       <c r="W32" s="57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X32" s="38" t="s">
         <v>74</v>
@@ -3761,7 +3761,7 @@
         <v>51</v>
       </c>
       <c r="O33" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P33" s="40" t="s">
         <v>51</v>
@@ -3893,7 +3893,7 @@
         <v>74</v>
       </c>
       <c r="U36" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V36" s="40" t="s">
         <v>51</v>
@@ -3999,10 +3999,10 @@
         <v>51</v>
       </c>
       <c r="G38" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H38" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I38" s="27" t="s">
         <v>51</v>
@@ -4047,7 +4047,7 @@
         <v>51</v>
       </c>
       <c r="W38" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X38" s="40" t="s">
         <v>51</v>
@@ -4224,7 +4224,7 @@
         <v>51</v>
       </c>
       <c r="H41" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I41" s="27" t="s">
         <v>51</v>
@@ -4269,7 +4269,7 @@
         <v>51</v>
       </c>
       <c r="W41" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X41" s="40" t="s">
         <v>51</v>
@@ -4375,7 +4375,7 @@
         <v>51</v>
       </c>
       <c r="I43" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J43" s="36" t="s">
         <v>51</v>
@@ -4396,10 +4396,10 @@
         <v>74</v>
       </c>
       <c r="P43" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q43" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R43" s="36" t="s">
         <v>51</v>
@@ -4440,7 +4440,7 @@
         <v>74</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G44" s="40" t="s">
         <v>51</v>
@@ -4470,16 +4470,16 @@
         <v>75</v>
       </c>
       <c r="P44" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q44" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R44" s="36" t="s">
         <v>51</v>
       </c>
       <c r="S44" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T44" s="19" t="s">
         <v>51</v>
@@ -4508,10 +4508,10 @@
         <v>47</v>
       </c>
       <c r="D45" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E45" s="61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F45" s="41" t="s">
         <v>51</v>
@@ -4565,7 +4565,7 @@
         <v>51</v>
       </c>
       <c r="W45" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X45" s="39" t="s">
         <v>51</v>
@@ -4615,7 +4615,7 @@
         <v>5</v>
       </c>
       <c r="O46" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P46" s="40" t="s">
         <v>75</v>
@@ -5201,7 +5201,7 @@
         <v>51</v>
       </c>
       <c r="M54" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N54" s="45" t="s">
         <v>51</v>
@@ -5248,7 +5248,7 @@
         <v>56</v>
       </c>
       <c r="D55" s="45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E55" s="45" t="s">
         <v>51</v>
@@ -5275,7 +5275,7 @@
         <v>51</v>
       </c>
       <c r="M55" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N55" s="45" t="s">
         <v>51</v>
@@ -5305,7 +5305,7 @@
         <v>51</v>
       </c>
       <c r="W55" s="55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X55" s="45" t="s">
         <v>51</v>
@@ -5775,7 +5775,7 @@
         <v>51</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H62" s="45" t="s">
         <v>51</v>
@@ -5808,7 +5808,7 @@
         <v>51</v>
       </c>
       <c r="R62" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S62" s="45" t="s">
         <v>51</v>
@@ -5855,7 +5855,7 @@
         <v>51</v>
       </c>
       <c r="I63" s="45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J63" s="45" t="s">
         <v>51</v>
@@ -5867,7 +5867,7 @@
         <v>51</v>
       </c>
       <c r="M63" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N63" s="45" t="s">
         <v>51</v>
@@ -5929,7 +5929,7 @@
         <v>51</v>
       </c>
       <c r="I64" s="45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J64" s="45" t="s">
         <v>51</v>
@@ -6151,7 +6151,7 @@
         <v>51</v>
       </c>
       <c r="I67" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J67" s="36" t="s">
         <v>51</v>
@@ -6163,13 +6163,13 @@
         <v>74</v>
       </c>
       <c r="M67" s="60" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N67" s="28" t="s">
         <v>5</v>
       </c>
       <c r="O67" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P67" s="40" t="s">
         <v>51</v>
@@ -6187,7 +6187,7 @@
         <v>51</v>
       </c>
       <c r="U67" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V67" s="36" t="s">
         <v>51</v>
@@ -6299,7 +6299,7 @@
         <v>51</v>
       </c>
       <c r="I69" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J69" s="36" t="s">
         <v>51</v>
@@ -6317,7 +6317,7 @@
         <v>5</v>
       </c>
       <c r="O69" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P69" s="40" t="s">
         <v>51</v>
@@ -6335,7 +6335,7 @@
         <v>51</v>
       </c>
       <c r="U69" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V69" s="36" t="s">
         <v>51</v>
@@ -6447,13 +6447,13 @@
         <v>51</v>
       </c>
       <c r="I71" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J71" s="36" t="s">
         <v>51</v>
       </c>
       <c r="K71" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L71" s="36" t="s">
         <v>51</v>
@@ -6465,7 +6465,7 @@
         <v>5</v>
       </c>
       <c r="O71" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P71" s="40" t="s">
         <v>51</v>
@@ -6595,7 +6595,7 @@
         <v>51</v>
       </c>
       <c r="I73" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J73" s="36" t="s">
         <v>51</v>
@@ -6613,7 +6613,7 @@
         <v>5</v>
       </c>
       <c r="O73" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P73" s="40" t="s">
         <v>51</v>
@@ -6752,7 +6752,7 @@
         <v>5</v>
       </c>
       <c r="L75" s="36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M75" s="28" t="s">
         <v>5</v>
@@ -6900,7 +6900,7 @@
         <v>5</v>
       </c>
       <c r="L77" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M77" s="28" t="s">
         <v>5</v>
@@ -7261,7 +7261,7 @@
         <v>51</v>
       </c>
       <c r="I82" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J82" s="36" t="s">
         <v>51</v>
@@ -7285,7 +7285,7 @@
         <v>51</v>
       </c>
       <c r="Q82" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R82" s="41" t="s">
         <v>51</v>
@@ -7329,7 +7329,7 @@
         <v>51</v>
       </c>
       <c r="G83" s="56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H83" s="40" t="s">
         <v>51</v>
@@ -19652,79 +19652,79 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>128</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>129</v>
       </c>
       <c r="R1" s="15" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AA1" s="14"/>
     </row>
     <row r="2" spans="1:27" ht="15">
       <c r="A2" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>88</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>51</v>
@@ -19793,13 +19793,13 @@
     </row>
     <row r="3" spans="1:27" ht="15">
       <c r="A3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="C3" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>51</v>
@@ -19868,13 +19868,13 @@
     </row>
     <row r="4" spans="1:27" ht="15">
       <c r="A4" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="C4" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>51</v>
@@ -19889,7 +19889,7 @@
         <v>51</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>51</v>
@@ -19898,7 +19898,7 @@
         <v>5</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L4" s="36" t="s">
         <v>51</v>
@@ -19916,10 +19916,10 @@
         <v>51</v>
       </c>
       <c r="Q4" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R4" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S4" s="40" t="s">
         <v>51</v>
@@ -19943,13 +19943,13 @@
     </row>
     <row r="5" spans="1:27" ht="15">
       <c r="A5" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>74</v>
@@ -19964,10 +19964,10 @@
         <v>75</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J5" s="40" t="s">
         <v>5</v>
@@ -19985,7 +19985,7 @@
         <v>74</v>
       </c>
       <c r="O5" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P5" s="40" t="s">
         <v>51</v>
@@ -20018,13 +20018,13 @@
     </row>
     <row r="6" spans="1:27" ht="15">
       <c r="A6" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="C6" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" s="41" t="s">
         <v>75</v>
@@ -20084,7 +20084,7 @@
         <v>51</v>
       </c>
       <c r="W6" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X6" s="40" t="s">
         <v>75</v>
@@ -20093,13 +20093,13 @@
     </row>
     <row r="7" spans="1:27" ht="15">
       <c r="A7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="C7" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="41" t="s">
         <v>75</v>
@@ -20108,7 +20108,7 @@
         <v>51</v>
       </c>
       <c r="F7" s="63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G7" s="40" t="s">
         <v>75</v>
@@ -20132,7 +20132,7 @@
         <v>74</v>
       </c>
       <c r="N7" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O7" s="27" t="s">
         <v>74</v>
@@ -20168,13 +20168,13 @@
     </row>
     <row r="8" spans="1:27" ht="15">
       <c r="A8" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="C8" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="41" t="s">
         <v>75</v>
@@ -20183,7 +20183,7 @@
         <v>51</v>
       </c>
       <c r="F8" s="63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" s="40" t="s">
         <v>75</v>
@@ -20207,7 +20207,7 @@
         <v>74</v>
       </c>
       <c r="N8" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O8" s="27" t="s">
         <v>74</v>
@@ -20243,13 +20243,13 @@
     </row>
     <row r="9" spans="1:27" s="48" customFormat="1" ht="15">
       <c r="A9" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="46" t="s">
         <v>95</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>96</v>
       </c>
       <c r="D9" s="47" t="s">
         <v>74</v>
@@ -20318,13 +20318,13 @@
     </row>
     <row r="10" spans="1:27" s="48" customFormat="1" ht="15">
       <c r="A10" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" s="47" t="s">
         <v>74</v>
@@ -20393,13 +20393,13 @@
     </row>
     <row r="11" spans="1:27" s="48" customFormat="1" ht="15">
       <c r="A11" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>75</v>
@@ -20468,13 +20468,13 @@
     </row>
     <row r="12" spans="1:27" s="48" customFormat="1" ht="15">
       <c r="A12" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>75</v>
@@ -20486,13 +20486,13 @@
         <v>5</v>
       </c>
       <c r="G12" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H12" s="48" t="s">
         <v>51</v>
       </c>
       <c r="I12" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J12" s="48" t="s">
         <v>5</v>
@@ -20504,25 +20504,25 @@
         <v>5</v>
       </c>
       <c r="M12" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N12" s="48" t="s">
         <v>51</v>
       </c>
       <c r="O12" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P12" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q12" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R12" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S12" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T12" s="48" t="s">
         <v>5</v>
@@ -20543,16 +20543,16 @@
     </row>
     <row r="13" spans="1:27" s="48" customFormat="1" ht="15">
       <c r="A13" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E13" s="48" t="s">
         <v>51</v>
@@ -20561,13 +20561,13 @@
         <v>5</v>
       </c>
       <c r="G13" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H13" s="48" t="s">
         <v>51</v>
       </c>
       <c r="I13" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J13" s="48" t="s">
         <v>5</v>
@@ -20579,34 +20579,34 @@
         <v>5</v>
       </c>
       <c r="M13" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N13" s="48" t="s">
         <v>51</v>
       </c>
       <c r="O13" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P13" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q13" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R13" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S13" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T13" s="48" t="s">
         <v>5</v>
       </c>
       <c r="U13" s="47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="V13" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="W13" s="48" t="s">
         <v>51</v>
@@ -20618,13 +20618,13 @@
     </row>
     <row r="14" spans="1:27" s="48" customFormat="1" ht="15">
       <c r="A14" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" s="47" t="s">
         <v>51</v>
@@ -20693,10 +20693,10 @@
     </row>
     <row r="15" spans="1:27" s="48" customFormat="1">
       <c r="A15" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="46" t="s">
         <v>84</v>
@@ -20738,7 +20738,7 @@
         <v>51</v>
       </c>
       <c r="P15" s="64" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q15" s="48" t="s">
         <v>51</v>
@@ -20768,10 +20768,10 @@
     </row>
     <row r="16" spans="1:27" s="48" customFormat="1">
       <c r="A16" s="67" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="67" t="s">
         <v>213</v>
-      </c>
-      <c r="B16" s="67" t="s">
-        <v>214</v>
       </c>
       <c r="C16" s="67" t="s">
         <v>15</v>
@@ -20843,13 +20843,13 @@
     </row>
     <row r="17" spans="1:27" s="48" customFormat="1">
       <c r="A17" s="67" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="67" t="s">
         <v>213</v>
       </c>
-      <c r="B17" s="67" t="s">
+      <c r="C17" s="67" t="s">
         <v>214</v>
-      </c>
-      <c r="C17" s="67" t="s">
-        <v>215</v>
       </c>
       <c r="D17" s="66" t="s">
         <v>74</v>
@@ -20918,13 +20918,13 @@
     </row>
     <row r="18" spans="1:27">
       <c r="A18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D18" s="16">
         <v>1</v>
@@ -20992,13 +20992,13 @@
     </row>
     <row r="19" spans="1:27" ht="15">
       <c r="A19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="D19" s="20">
         <v>0</v>
@@ -21067,13 +21067,13 @@
     </row>
     <row r="20" spans="1:27" ht="15">
       <c r="A20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" s="20">
         <v>0</v>
@@ -21142,13 +21142,13 @@
     </row>
     <row r="21" spans="1:27" ht="15">
       <c r="A21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" s="20">
         <v>0</v>
@@ -21217,13 +21217,13 @@
     </row>
     <row r="22" spans="1:27" ht="15">
       <c r="A22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" s="20">
         <v>0</v>
@@ -21292,13 +21292,13 @@
     </row>
     <row r="23" spans="1:27" ht="15">
       <c r="A23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" s="20">
         <v>0</v>
@@ -21367,13 +21367,13 @@
     </row>
     <row r="24" spans="1:27" ht="15">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D24" s="20">
         <v>1</v>
@@ -21441,13 +21441,13 @@
     </row>
     <row r="25" spans="1:27" ht="15">
       <c r="A25" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D25" s="20">
         <v>0</v>
@@ -21515,13 +21515,13 @@
     </row>
     <row r="26" spans="1:27" ht="15">
       <c r="A26" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D26" s="20">
         <v>0</v>
@@ -21589,13 +21589,13 @@
     </row>
     <row r="27" spans="1:27" ht="15">
       <c r="A27" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D27" s="20">
         <v>0</v>
@@ -21663,13 +21663,13 @@
     </row>
     <row r="28" spans="1:27" ht="15">
       <c r="A28" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D28" s="20">
         <v>0</v>
@@ -21740,7 +21740,7 @@
     </row>
     <row r="30" spans="1:27">
       <c r="A30" s="46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D30" s="36"/>
       <c r="E30" s="36"/>
@@ -21753,7 +21753,7 @@
     </row>
     <row r="32" spans="1:27">
       <c r="A32" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:1">
@@ -21808,33 +21808,33 @@
         <v>2</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I1" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="K1" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="J1" s="33" t="s">
-        <v>195</v>
-      </c>
-      <c r="K1" s="33" t="s">
-        <v>127</v>
-      </c>
       <c r="L1" s="33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>51</v>
@@ -21846,16 +21846,16 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I3" s="32"/>
       <c r="J3" s="32"/>
@@ -21864,13 +21864,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>75</v>
@@ -21882,13 +21882,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" s="30" t="s">
         <v>74</v>
@@ -21903,25 +21903,25 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="D6" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I6" s="32" t="s">
         <v>74</v>
       </c>
       <c r="J6" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K6" s="32" t="s">
         <v>74</v>
       </c>
       <c r="L6" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -21929,19 +21929,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I7" s="32" t="s">
         <v>74</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K7" s="32" t="s">
         <v>74</v>
@@ -21953,10 +21953,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>75</v>
@@ -21975,10 +21975,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>74</v>
@@ -21997,10 +21997,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>51</v>
@@ -22011,16 +22011,16 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I11" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -22028,13 +22028,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -22042,13 +22042,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -22056,10 +22056,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>75</v>
@@ -22070,10 +22070,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>75</v>
@@ -22084,10 +22084,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>75</v>
@@ -22098,10 +22098,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>75</v>
@@ -22112,10 +22112,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>74</v>
@@ -22126,10 +22126,10 @@
         <v>3</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>74</v>
@@ -22140,7 +22140,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" s="35">
         <v>1</v>
@@ -22154,13 +22154,13 @@
         <v>3</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="D21" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -22168,13 +22168,13 @@
         <v>3</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -22182,10 +22182,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>75</v>
@@ -22196,10 +22196,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>75</v>
@@ -22210,10 +22210,10 @@
         <v>3</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>74</v>
@@ -22224,10 +22224,10 @@
         <v>3</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>162</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>51</v>
@@ -22238,13 +22238,13 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -22252,13 +22252,13 @@
         <v>3</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -22266,10 +22266,10 @@
         <v>3</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D29" s="21" t="s">
         <v>75</v>
@@ -22280,10 +22280,10 @@
         <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D30" s="21" t="s">
         <v>74</v>
@@ -22294,10 +22294,10 @@
         <v>3</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>168</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>51</v>
@@ -22308,13 +22308,13 @@
         <v>3</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -22322,13 +22322,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -22336,10 +22336,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D34" s="24" t="s">
         <v>75</v>
@@ -22350,10 +22350,10 @@
         <v>3</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>75</v>
@@ -22364,10 +22364,10 @@
         <v>3</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>74</v>
@@ -22378,10 +22378,10 @@
         <v>3</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D37" s="24" t="s">
         <v>74</v>
@@ -22392,10 +22392,10 @@
         <v>3</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="D38" s="21" t="s">
         <v>51</v>
@@ -22406,10 +22406,10 @@
         <v>3</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D39" s="21" t="s">
         <v>75</v>
@@ -22420,10 +22420,10 @@
         <v>3</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D40" s="21" t="s">
         <v>74</v>
@@ -22434,10 +22434,10 @@
         <v>3</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>177</v>
       </c>
       <c r="D41" s="24" t="s">
         <v>51</v>
@@ -22448,13 +22448,13 @@
         <v>3</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -22462,10 +22462,10 @@
         <v>3</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>75</v>
@@ -22476,10 +22476,10 @@
         <v>3</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D44" s="24" t="s">
         <v>75</v>
@@ -22490,7 +22490,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>5</v>
@@ -22504,10 +22504,10 @@
         <v>3</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>51</v>
@@ -22518,13 +22518,13 @@
         <v>3</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -22532,10 +22532,10 @@
         <v>3</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D48" s="21" t="s">
         <v>75</v>
@@ -22546,10 +22546,10 @@
         <v>3</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D49" s="21" t="s">
         <v>75</v>
@@ -22560,10 +22560,10 @@
         <v>3</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D50" s="21" t="s">
         <v>74</v>
@@ -22574,7 +22574,7 @@
         <v>3</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>15</v>
@@ -22588,7 +22588,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>16</v>
@@ -22599,13 +22599,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B53" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="D53" s="25" t="s">
         <v>51</v>
@@ -22613,27 +22613,27 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D55" s="25" t="s">
         <v>74</v>
@@ -22641,13 +22641,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>74</v>
@@ -22655,10 +22655,10 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>5</v>
@@ -22669,10 +22669,10 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>15</v>
@@ -22683,10 +22683,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>16</v>
@@ -22697,13 +22697,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D60" s="32" t="s">
         <v>51</v>
@@ -22711,27 +22711,27 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D62" s="32" t="s">
         <v>74</v>
@@ -22739,10 +22739,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C63" s="31" t="s">
         <v>5</v>
@@ -22753,10 +22753,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C64" s="31" t="s">
         <v>15</v>
@@ -22767,10 +22767,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C65" s="31" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
just rewriting the damn feeding larva trait values - this time dropping the hyphen
Former-commit-id: 714b9d3845f0fe39fb3c2e6df5fb27e5ceb11f4a
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -698,19 +698,19 @@
     <t xml:space="preserve">no </t>
   </si>
   <si>
-    <t>feeding -calcifier</t>
+    <t>no larva</t>
   </si>
   <si>
-    <t>feeding - non-calcifier</t>
+    <t>feeding calcifier</t>
   </si>
   <si>
-    <t>non-feeding - calcifier</t>
+    <t>feeding non-calcifier</t>
   </si>
   <si>
-    <t>non-feeding - non-calcifier</t>
+    <t>non-feeding calcifier</t>
   </si>
   <si>
-    <t>no larva</t>
+    <t>non-feeding non-calcifier</t>
   </si>
 </sst>
 </file>
@@ -1015,11 +1015,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1311,7 +1311,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1431,7 +1431,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>5</v>
@@ -1505,7 +1505,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>5</v>
@@ -1579,7 +1579,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>5</v>
@@ -1653,7 +1653,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D5" s="36" t="s">
         <v>5</v>
@@ -1727,7 +1727,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
updating spp and stressor trait sheets to re-run
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Dropbox\Fiji_workshop_after\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F19E4B-AE6E-4DD8-97B1-44A4E917CD1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD3FBD7-F5A1-4550-94E9-0214C9C04FEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="510" windowWidth="20490" windowHeight="14625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7725" yWindow="735" windowWidth="17820" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensitivity" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="gen_adcap" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="sens_traits" localSheetId="0">sensitivity!$A$4:$C$98</definedName>
-    <definedName name="sens_traits_1" localSheetId="0">sensitivity!$A$4:$C$84</definedName>
+    <definedName name="sens_traits" localSheetId="0">sensitivity!$A$4:$C$100</definedName>
+    <definedName name="sens_traits_1" localSheetId="0">sensitivity!$A$4:$C$86</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2671" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="221">
   <si>
     <t>category</t>
   </si>
@@ -718,6 +718,9 @@
   <si>
     <t>no larva</t>
   </si>
+  <si>
+    <t>habitat forming</t>
+  </si>
 </sst>
 </file>
 
@@ -784,7 +787,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -893,6 +896,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -909,7 +918,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1003,6 +1012,11 @@
     <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1030,11 +1044,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="sens_traits" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="sens_traits_1" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="sens_traits_1" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="sens_traits" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1334,14 +1348,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB3729"/>
+  <dimension ref="A1:AB3731"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3500,8 +3514,8 @@
       <c r="U29" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="V29" s="40" t="s">
-        <v>75</v>
+      <c r="V29" s="71" t="s">
+        <v>74</v>
       </c>
       <c r="W29" s="40" t="s">
         <v>51</v>
@@ -3846,166 +3860,162 @@
       <c r="P35" s="40"/>
       <c r="W35" s="53"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="7" t="s">
+    <row r="36" spans="1:24" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="73" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="69" t="s">
+      <c r="D36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="E36" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F36" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="G36" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H36" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="I36" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="J36" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="K36" s="65" t="s">
-        <v>75</v>
-      </c>
-      <c r="L36" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M36" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="N36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="O36" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="P36" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q36" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="R36" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="S36" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="T36" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="U36" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="V36" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="W36" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="X36" s="40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="7" t="s">
+      <c r="I36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="K36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="L36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="M36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="N36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="O36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="P36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="R36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="S36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="T36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="U36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="V36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="W36" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="X36" s="71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="73" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F37" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="G37" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H37" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="I37" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="J37" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="K37" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L37" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M37" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="N37" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="O37" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="P37" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q37" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="R37" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="S37" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="T37" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U37" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="V37" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="W37" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="X37" s="40" t="s">
-        <v>51</v>
+      <c r="D37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="J37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="L37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="M37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="N37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="O37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="P37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="R37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="S37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="T37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="U37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="V37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="W37" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="X37" s="71" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="40" t="s">
-        <v>5</v>
+      <c r="B38" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="69" t="s">
+        <v>74</v>
       </c>
       <c r="E38" s="40" t="s">
         <v>51</v>
@@ -4013,56 +4023,56 @@
       <c r="F38" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="G38" s="56" t="s">
+      <c r="G38" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H38" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="J38" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K38" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="L38" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="M38" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="N38" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="O38" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="P38" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q38" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="R38" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="S38" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="T38" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="U38" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="H38" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="I38" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="J38" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="K38" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L38" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M38" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="N38" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="O38" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="P38" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q38" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="R38" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="S38" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="T38" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U38" s="36" t="s">
-        <v>51</v>
-      </c>
       <c r="V38" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="W38" s="40" t="s">
-        <v>132</v>
+      <c r="W38" s="56" t="s">
+        <v>75</v>
       </c>
       <c r="X38" s="40" t="s">
         <v>51</v>
@@ -4072,14 +4082,14 @@
       <c r="A39" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="40" t="s">
-        <v>5</v>
+      <c r="B39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="56" t="s">
+        <v>51</v>
       </c>
       <c r="E39" s="40" t="s">
         <v>51</v>
@@ -4114,8 +4124,8 @@
       <c r="O39" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="P39" s="27" t="s">
-        <v>5</v>
+      <c r="P39" s="40" t="s">
+        <v>51</v>
       </c>
       <c r="Q39" s="40" t="s">
         <v>51</v>
@@ -4135,7 +4145,7 @@
       <c r="V39" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="W39" s="40" t="s">
+      <c r="W39" s="56" t="s">
         <v>51</v>
       </c>
       <c r="X39" s="40" t="s">
@@ -4150,34 +4160,34 @@
         <v>39</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D40" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G40" s="27" t="s">
-        <v>5</v>
+      <c r="E40" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G40" s="56" t="s">
+        <v>132</v>
       </c>
       <c r="H40" s="36" t="s">
-        <v>5</v>
+        <v>132</v>
       </c>
       <c r="I40" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J40" s="17" t="s">
-        <v>5</v>
+        <v>51</v>
+      </c>
+      <c r="J40" s="36" t="s">
+        <v>51</v>
       </c>
       <c r="K40" s="19" t="s">
         <v>5</v>
       </c>
       <c r="L40" s="36" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="M40" s="19" t="s">
         <v>5</v>
@@ -4186,31 +4196,31 @@
         <v>5</v>
       </c>
       <c r="O40" s="27" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="P40" s="27" t="s">
         <v>5</v>
       </c>
       <c r="Q40" s="40" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="R40" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="S40" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="T40" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="U40" s="8" t="s">
-        <v>5</v>
+        <v>51</v>
+      </c>
+      <c r="S40" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="T40" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="U40" s="36" t="s">
+        <v>51</v>
       </c>
       <c r="V40" s="40" t="s">
         <v>51</v>
       </c>
       <c r="W40" s="40" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="X40" s="40" t="s">
         <v>51</v>
@@ -4220,11 +4230,11 @@
       <c r="A41" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>15</v>
+      <c r="B41" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="D41" s="40" t="s">
         <v>5</v>
@@ -4239,7 +4249,7 @@
         <v>51</v>
       </c>
       <c r="H41" s="36" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="I41" s="27" t="s">
         <v>51</v>
@@ -4284,7 +4294,7 @@
         <v>51</v>
       </c>
       <c r="W41" s="40" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="X41" s="40" t="s">
         <v>51</v>
@@ -4294,168 +4304,168 @@
       <c r="A42" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="I42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K42" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L42" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="M42" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="N42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="O42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="P42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="R42" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="S42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="T42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="U42" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="V42" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="W42" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="X42" s="40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C43" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F43" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G43" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H43" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="I43" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="J43" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K43" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L43" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="M43" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="N43" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="O43" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="P43" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q43" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="R43" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="S43" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="T43" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="U43" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="V43" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="W43" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="X43" s="40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="G42" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H42" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="I42" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="J42" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="K42" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L42" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M42" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="N42" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="O42" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="P42" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q42" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="R42" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="S42" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="T42" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U42" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="V42" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="W42" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="X42" s="40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="E43" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="F43" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="G43" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H43" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="I43" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="J43" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="K43" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L43" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M43" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="N43" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="O43" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="P43" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q43" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="R43" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="S43" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="T43" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U43" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="V43" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="W43" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="X43" s="39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" s="54" t="s">
-        <v>51</v>
+      <c r="D44" s="40" t="s">
+        <v>5</v>
       </c>
       <c r="E44" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="F44" s="41" t="s">
-        <v>132</v>
+        <v>51</v>
+      </c>
+      <c r="F44" s="40" t="s">
+        <v>51</v>
       </c>
       <c r="G44" s="40" t="s">
         <v>51</v>
@@ -4464,7 +4474,7 @@
         <v>51</v>
       </c>
       <c r="I44" s="27" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="J44" s="36" t="s">
         <v>51</v>
@@ -4482,19 +4492,19 @@
         <v>5</v>
       </c>
       <c r="O44" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="P44" s="40" t="s">
-        <v>132</v>
+        <v>51</v>
+      </c>
+      <c r="P44" s="27" t="s">
+        <v>5</v>
       </c>
       <c r="Q44" s="40" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="R44" s="36" t="s">
         <v>51</v>
       </c>
       <c r="S44" s="40" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="T44" s="19" t="s">
         <v>51</v>
@@ -4508,8 +4518,8 @@
       <c r="W44" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="X44" s="68" t="s">
-        <v>75</v>
+      <c r="X44" s="40" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -4520,55 +4530,55 @@
         <v>44</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D45" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="F45" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H45" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I45" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="E45" s="61" t="s">
+      <c r="J45" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K45" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L45" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="M45" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="N45" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="O45" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="P45" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="F45" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="G45" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H45" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="I45" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="J45" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="K45" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L45" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M45" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="N45" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="O45" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="P45" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q45" s="52" t="s">
-        <v>75</v>
+      <c r="Q45" s="40" t="s">
+        <v>132</v>
       </c>
       <c r="R45" s="36" t="s">
         <v>51</v>
       </c>
       <c r="S45" s="40" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="T45" s="19" t="s">
         <v>51</v>
@@ -4580,10 +4590,10 @@
         <v>51</v>
       </c>
       <c r="W45" s="40" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="X45" s="39" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -4594,26 +4604,26 @@
         <v>44</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D46" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="G46" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H46" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I46" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="E46" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F46" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="G46" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H46" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="I46" s="27" t="s">
-        <v>74</v>
-      </c>
       <c r="J46" s="36" t="s">
         <v>51</v>
       </c>
@@ -4623,41 +4633,41 @@
       <c r="L46" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="M46" s="28" t="s">
+      <c r="M46" s="19" t="s">
         <v>5</v>
       </c>
       <c r="N46" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="O46" s="58" t="s">
+      <c r="O46" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="P46" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="P46" s="40" t="s">
+      <c r="Q46" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="R46" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="S46" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="T46" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="U46" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="V46" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="W46" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="X46" s="68" t="s">
         <v>75</v>
-      </c>
-      <c r="Q46" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="R46" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="S46" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="T46" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U46" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="V46" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="W46" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="X46" s="39" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -4668,84 +4678,84 @@
         <v>44</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="27" t="s">
-        <v>5</v>
+        <v>47</v>
+      </c>
+      <c r="D47" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="E47" s="61" t="s">
+        <v>132</v>
       </c>
       <c r="F47" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="G47" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H47" s="27" t="s">
-        <v>5</v>
+        <v>51</v>
+      </c>
+      <c r="G47" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H47" s="36" t="s">
+        <v>51</v>
       </c>
       <c r="I47" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J47" s="17" t="s">
-        <v>5</v>
+        <v>75</v>
+      </c>
+      <c r="J47" s="36" t="s">
+        <v>51</v>
       </c>
       <c r="K47" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="L47" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="M47" s="28" t="s">
+      <c r="L47" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="M47" s="19" t="s">
         <v>5</v>
       </c>
       <c r="N47" s="27" t="s">
         <v>5</v>
       </c>
       <c r="O47" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="P47" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q47" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="R47" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="S47" s="27" t="s">
-        <v>5</v>
+        <v>75</v>
+      </c>
+      <c r="P47" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q47" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="R47" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="S47" s="40" t="s">
+        <v>75</v>
       </c>
       <c r="T47" s="19" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="U47" s="36" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="V47" s="40" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="W47" s="40" t="s">
-        <v>5</v>
+        <v>132</v>
       </c>
       <c r="X47" s="39" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="40" t="s">
-        <v>5</v>
+        <v>48</v>
+      </c>
+      <c r="D48" s="54" t="s">
+        <v>75</v>
       </c>
       <c r="E48" s="40" t="s">
         <v>51</v>
@@ -4753,280 +4763,280 @@
       <c r="F48" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="G48" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="H48" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I48" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="J48" s="40" t="s">
+      <c r="G48" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H48" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I48" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="J48" s="36" t="s">
         <v>51</v>
       </c>
       <c r="K48" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="L48" s="40" t="s">
+      <c r="L48" s="36" t="s">
         <v>51</v>
       </c>
       <c r="M48" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="N48" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="O48" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="P48" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q48" s="41" t="s">
-        <v>51</v>
+      <c r="N48" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="O48" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="P48" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q48" s="40" t="s">
+        <v>74</v>
       </c>
       <c r="R48" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="S48" s="41" t="s">
-        <v>51</v>
+      <c r="S48" s="40" t="s">
+        <v>75</v>
       </c>
       <c r="T48" s="19" t="s">
         <v>51</v>
       </c>
       <c r="U48" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="V48" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="W48" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="V48" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="W48" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="X48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X48" s="39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B49" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I49" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J49" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K49" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="M49" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N49" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="O49" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="P49" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q49" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="R49" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="S49" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="T49" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="U49" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="V49" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="W49" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="X49" s="39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C50" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F50" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I50" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="J50" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="K50" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L50" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="M50" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N50" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O50" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="P50" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q50" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="R50" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="S50" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="T50" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="U50" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="V50" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="W50" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="X50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F49" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="G49" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I49" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="J49" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="K49" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L49" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="M49" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="N49" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="O49" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="P49" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q49" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="R49" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="S49" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="T49" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U49" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="V49" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="W49" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="X49" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D50" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I50" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="J50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="L50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="M50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="N50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="O50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="P50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="R50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="S50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="T50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="U50" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="V50" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="W50" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="X50" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="E51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="F51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="I51" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="J51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="K51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="L51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="M51" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="N51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="O51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="P51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="R51" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="S51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="T51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="U51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="V51" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="W51" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="X51" s="45" t="s">
+      <c r="D51" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F51" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="G51" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I51" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="J51" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="K51" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L51" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="M51" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N51" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O51" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="P51" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q51" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="R51" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="S51" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="T51" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="U51" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="V51" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="W51" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="X51" t="s">
         <v>51</v>
       </c>
     </row>
@@ -5038,69 +5048,69 @@
         <v>50</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D52" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="E52" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="F52" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F52" s="12" t="s">
         <v>51</v>
       </c>
       <c r="G52" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H52" s="45" t="s">
+      <c r="H52" s="12" t="s">
         <v>51</v>
       </c>
       <c r="I52" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="J52" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="K52" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="L52" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L52" s="12" t="s">
         <v>51</v>
       </c>
       <c r="M52" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="N52" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="O52" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="P52" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q52" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="P52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q52" s="12" t="s">
         <v>51</v>
       </c>
       <c r="R52" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="S52" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="T52" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="U52" s="45" t="s">
+      <c r="S52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="T52" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="U52" s="12" t="s">
         <v>51</v>
       </c>
       <c r="V52" s="45" t="s">
         <v>51</v>
       </c>
       <c r="W52" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="X52" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="X52" s="12" t="s">
         <v>51</v>
       </c>
     </row>
@@ -5112,7 +5122,7 @@
         <v>50</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D53" s="45" t="s">
         <v>75</v>
@@ -5123,8 +5133,8 @@
       <c r="F53" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="G53" s="45" t="s">
-        <v>74</v>
+      <c r="G53" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="H53" s="45" t="s">
         <v>51</v>
@@ -5142,7 +5152,7 @@
         <v>51</v>
       </c>
       <c r="M53" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N53" s="45" t="s">
         <v>51</v>
@@ -5157,7 +5167,7 @@
         <v>51</v>
       </c>
       <c r="R53" s="12" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="S53" s="45" t="s">
         <v>51</v>
@@ -5178,7 +5188,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:24" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>43</v>
       </c>
@@ -5186,7 +5196,7 @@
         <v>50</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D54" s="45" t="s">
         <v>75</v>
@@ -5204,7 +5214,7 @@
         <v>51</v>
       </c>
       <c r="I54" s="45" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="J54" s="45" t="s">
         <v>51</v>
@@ -5215,8 +5225,8 @@
       <c r="L54" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M54" s="58" t="s">
-        <v>132</v>
+      <c r="M54" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="N54" s="45" t="s">
         <v>51</v>
@@ -5252,7 +5262,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:24" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>43</v>
       </c>
@@ -5260,10 +5270,10 @@
         <v>50</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D55" s="45" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="E55" s="45" t="s">
         <v>51</v>
@@ -5271,14 +5281,14 @@
       <c r="F55" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="G55" s="12" t="s">
-        <v>51</v>
+      <c r="G55" s="45" t="s">
+        <v>74</v>
       </c>
       <c r="H55" s="45" t="s">
         <v>51</v>
       </c>
       <c r="I55" s="45" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="J55" s="45" t="s">
         <v>51</v>
@@ -5289,8 +5299,8 @@
       <c r="L55" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M55" s="58" t="s">
-        <v>132</v>
+      <c r="M55" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="N55" s="45" t="s">
         <v>51</v>
@@ -5305,7 +5315,7 @@
         <v>51</v>
       </c>
       <c r="R55" s="12" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="S55" s="45" t="s">
         <v>51</v>
@@ -5320,24 +5330,24 @@
         <v>51</v>
       </c>
       <c r="W55" s="55" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="X55" s="45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D56" s="45" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="E56" s="45" t="s">
         <v>51</v>
@@ -5345,7 +5355,7 @@
       <c r="F56" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="G56" s="45" t="s">
+      <c r="G56" s="12" t="s">
         <v>51</v>
       </c>
       <c r="H56" s="45" t="s">
@@ -5363,8 +5373,8 @@
       <c r="L56" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M56" s="45" t="s">
-        <v>51</v>
+      <c r="M56" s="58" t="s">
+        <v>132</v>
       </c>
       <c r="N56" s="45" t="s">
         <v>51</v>
@@ -5378,7 +5388,7 @@
       <c r="Q56" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="R56" s="45" t="s">
+      <c r="R56" s="12" t="s">
         <v>51</v>
       </c>
       <c r="S56" s="45" t="s">
@@ -5394,24 +5404,24 @@
         <v>51</v>
       </c>
       <c r="W56" s="55" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="X56" s="45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D57" s="45" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="E57" s="45" t="s">
         <v>51</v>
@@ -5419,14 +5429,14 @@
       <c r="F57" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="G57" s="45" t="s">
-        <v>74</v>
+      <c r="G57" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="H57" s="45" t="s">
         <v>51</v>
       </c>
       <c r="I57" s="45" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="J57" s="45" t="s">
         <v>51</v>
@@ -5437,8 +5447,8 @@
       <c r="L57" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M57" s="45" t="s">
-        <v>74</v>
+      <c r="M57" s="58" t="s">
+        <v>132</v>
       </c>
       <c r="N57" s="45" t="s">
         <v>51</v>
@@ -5452,8 +5462,8 @@
       <c r="Q57" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="R57" s="45" t="s">
-        <v>74</v>
+      <c r="R57" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="S57" s="45" t="s">
         <v>51</v>
@@ -5468,7 +5478,7 @@
         <v>51</v>
       </c>
       <c r="W57" s="55" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="X57" s="45" t="s">
         <v>51</v>
@@ -5482,10 +5492,10 @@
         <v>57</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D58" s="45" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="E58" s="45" t="s">
         <v>51</v>
@@ -5494,13 +5504,13 @@
         <v>51</v>
       </c>
       <c r="G58" s="45" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="H58" s="45" t="s">
         <v>51</v>
       </c>
       <c r="I58" s="45" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="J58" s="45" t="s">
         <v>51</v>
@@ -5512,7 +5522,7 @@
         <v>51</v>
       </c>
       <c r="M58" s="45" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="N58" s="45" t="s">
         <v>51</v>
@@ -5527,7 +5537,7 @@
         <v>51</v>
       </c>
       <c r="R58" s="45" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="S58" s="45" t="s">
         <v>51</v>
@@ -5542,7 +5552,7 @@
         <v>51</v>
       </c>
       <c r="W58" s="55" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="X58" s="45" t="s">
         <v>51</v>
@@ -5556,7 +5566,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D59" s="45" t="s">
         <v>74</v>
@@ -5627,10 +5637,10 @@
         <v>43</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D60" s="45" t="s">
         <v>75</v>
@@ -5641,7 +5651,7 @@
       <c r="F60" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="G60" s="12" t="s">
+      <c r="G60" s="45" t="s">
         <v>75</v>
       </c>
       <c r="H60" s="45" t="s">
@@ -5659,7 +5669,7 @@
       <c r="L60" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M60" s="12" t="s">
+      <c r="M60" s="45" t="s">
         <v>74</v>
       </c>
       <c r="N60" s="45" t="s">
@@ -5674,7 +5684,7 @@
       <c r="Q60" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="R60" s="12" t="s">
+      <c r="R60" s="45" t="s">
         <v>75</v>
       </c>
       <c r="S60" s="45" t="s">
@@ -5701,10 +5711,10 @@
         <v>43</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D61" s="45" t="s">
         <v>74</v>
@@ -5715,14 +5725,14 @@
       <c r="F61" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="G61" s="12" t="s">
-        <v>75</v>
+      <c r="G61" s="45" t="s">
+        <v>74</v>
       </c>
       <c r="H61" s="45" t="s">
         <v>51</v>
       </c>
       <c r="I61" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J61" s="45" t="s">
         <v>51</v>
@@ -5733,7 +5743,7 @@
       <c r="L61" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M61" s="12" t="s">
+      <c r="M61" s="45" t="s">
         <v>74</v>
       </c>
       <c r="N61" s="45" t="s">
@@ -5748,8 +5758,8 @@
       <c r="Q61" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="R61" s="12" t="s">
-        <v>75</v>
+      <c r="R61" s="45" t="s">
+        <v>74</v>
       </c>
       <c r="S61" s="45" t="s">
         <v>51</v>
@@ -5778,7 +5788,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D62" s="45" t="s">
         <v>75</v>
@@ -5790,7 +5800,7 @@
         <v>51</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="H62" s="45" t="s">
         <v>51</v>
@@ -5808,22 +5818,22 @@
         <v>51</v>
       </c>
       <c r="M62" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="N62" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="O62" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="P62" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q62" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="R62" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="N62" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="O62" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="P62" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q62" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="R62" s="12" t="s">
-        <v>132</v>
       </c>
       <c r="S62" s="45" t="s">
         <v>51</v>
@@ -5852,25 +5862,25 @@
         <v>61</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D63" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="E63" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="F63" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="G63" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E63" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="F63" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="H63" s="45" t="s">
         <v>51</v>
       </c>
       <c r="I63" s="45" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="J63" s="45" t="s">
         <v>51</v>
@@ -5882,7 +5892,7 @@
         <v>51</v>
       </c>
       <c r="M63" s="12" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="N63" s="45" t="s">
         <v>51</v>
@@ -5897,7 +5907,7 @@
         <v>51</v>
       </c>
       <c r="R63" s="12" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="S63" s="45" t="s">
         <v>51</v>
@@ -5912,7 +5922,7 @@
         <v>51</v>
       </c>
       <c r="W63" s="55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X63" s="45" t="s">
         <v>51</v>
@@ -5926,7 +5936,7 @@
         <v>61</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D64" s="45" t="s">
         <v>75</v>
@@ -5938,40 +5948,40 @@
         <v>51</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="H64" s="45" t="s">
         <v>51</v>
       </c>
       <c r="I64" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="J64" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="K64" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="L64" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="M64" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N64" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="O64" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="P64" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q64" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="R64" s="12" t="s">
         <v>132</v>
-      </c>
-      <c r="J64" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="K64" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="L64" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="M64" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="N64" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="O64" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="P64" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q64" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="R64" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="S64" s="45" t="s">
         <v>51</v>
@@ -6000,7 +6010,7 @@
         <v>61</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D65" s="45" t="s">
         <v>75</v>
@@ -6018,7 +6028,7 @@
         <v>51</v>
       </c>
       <c r="I65" s="45" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="J65" s="45" t="s">
         <v>51</v>
@@ -6030,7 +6040,7 @@
         <v>51</v>
       </c>
       <c r="M65" s="12" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="N65" s="45" t="s">
         <v>51</v>
@@ -6074,10 +6084,10 @@
         <v>61</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D66" s="45" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="E66" s="45" t="s">
         <v>51</v>
@@ -6092,7 +6102,7 @@
         <v>51</v>
       </c>
       <c r="I66" s="45" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="J66" s="45" t="s">
         <v>51</v>
@@ -6134,157 +6144,157 @@
         <v>51</v>
       </c>
       <c r="W66" s="55" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="X66" s="45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
+    <row r="67" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B67" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E67" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F67" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="G67" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H67" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="I67" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="J67" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="K67" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L67" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="M67" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="N67" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="O67" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="P67" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q67" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="R67" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="S67" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="T67" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U67" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="V67" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="W67" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="X67" s="41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
+      <c r="B67" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="E67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="F67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="I67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="J67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="K67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="L67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="M67" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="O67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="P67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="R67" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="S67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="T67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="U67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="V67" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="W67" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="X67" s="45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B68" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D68" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E68" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F68" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="G68" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H68" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="I68" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="J68" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="K68" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L68" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M68" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="N68" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="O68" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="P68" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q68" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="R68" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="S68" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="T68" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U68" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="V68" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="W68" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="X68" s="41" t="s">
+      <c r="B68" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="F68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="I68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="J68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="K68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="L68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="M68" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="O68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="P68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="R68" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="S68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="T68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="U68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="V68" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="W68" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="X68" s="45" t="s">
         <v>51</v>
       </c>
     </row>
@@ -6292,10 +6302,10 @@
       <c r="A69" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B69" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69" s="9" t="s">
+      <c r="B69" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C69" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D69" s="40" t="s">
@@ -6325,8 +6335,8 @@
       <c r="L69" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="M69" s="28" t="s">
-        <v>5</v>
+      <c r="M69" s="60" t="s">
+        <v>132</v>
       </c>
       <c r="N69" s="28" t="s">
         <v>5</v>
@@ -6366,10 +6376,10 @@
       <c r="A70" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B70" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" s="9" t="s">
+      <c r="B70" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D70" s="40" t="s">
@@ -6440,10 +6450,10 @@
       <c r="A71" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B71" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C71" s="11" t="s">
+      <c r="B71" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D71" s="40" t="s">
@@ -6456,7 +6466,7 @@
         <v>51</v>
       </c>
       <c r="G71" s="40" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="H71" s="40" t="s">
         <v>51</v>
@@ -6467,11 +6477,11 @@
       <c r="J71" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="K71" s="56" t="s">
-        <v>132</v>
+      <c r="K71" s="19" t="s">
+        <v>5</v>
       </c>
       <c r="L71" s="36" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="M71" s="28" t="s">
         <v>5</v>
@@ -6492,13 +6502,13 @@
         <v>51</v>
       </c>
       <c r="S71" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="T71" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="U71" s="36" t="s">
-        <v>51</v>
+        <v>51</v>
+      </c>
+      <c r="T71" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="U71" s="40" t="s">
+        <v>132</v>
       </c>
       <c r="V71" s="36" t="s">
         <v>51</v>
@@ -6514,10 +6524,10 @@
       <c r="A72" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B72" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C72" s="11" t="s">
+      <c r="B72" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D72" s="40" t="s">
@@ -6542,7 +6552,7 @@
         <v>51</v>
       </c>
       <c r="K72" s="19" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="L72" s="36" t="s">
         <v>51</v>
@@ -6571,7 +6581,7 @@
       <c r="T72" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="U72" s="36" t="s">
+      <c r="U72" s="40" t="s">
         <v>51</v>
       </c>
       <c r="V72" s="36" t="s">
@@ -6588,10 +6598,10 @@
       <c r="A73" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B73" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C73" s="9" t="s">
+      <c r="B73" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D73" s="40" t="s">
@@ -6604,7 +6614,7 @@
         <v>51</v>
       </c>
       <c r="G73" s="40" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="H73" s="40" t="s">
         <v>51</v>
@@ -6615,8 +6625,8 @@
       <c r="J73" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="K73" s="19" t="s">
-        <v>5</v>
+      <c r="K73" s="56" t="s">
+        <v>132</v>
       </c>
       <c r="L73" s="36" t="s">
         <v>51</v>
@@ -6640,10 +6650,10 @@
         <v>51</v>
       </c>
       <c r="S73" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="T73" s="19" t="s">
-        <v>51</v>
+        <v>74</v>
+      </c>
+      <c r="T73" s="40" t="s">
+        <v>74</v>
       </c>
       <c r="U73" s="36" t="s">
         <v>51</v>
@@ -6658,14 +6668,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="74" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B74" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C74" s="9" t="s">
+      <c r="B74" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D74" s="40" t="s">
@@ -6683,14 +6693,14 @@
       <c r="H74" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="I74" s="27" t="s">
+      <c r="I74" s="53" t="s">
         <v>51</v>
       </c>
       <c r="J74" s="36" t="s">
         <v>51</v>
       </c>
       <c r="K74" s="19" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="L74" s="36" t="s">
         <v>51</v>
@@ -6736,11 +6746,11 @@
       <c r="A75" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B75" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>74</v>
+      <c r="B75" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="D75" s="40" t="s">
         <v>51</v>
@@ -6758,7 +6768,7 @@
         <v>51</v>
       </c>
       <c r="I75" s="58" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="J75" s="36" t="s">
         <v>51</v>
@@ -6767,7 +6777,7 @@
         <v>5</v>
       </c>
       <c r="L75" s="36" t="s">
-        <v>202</v>
+        <v>51</v>
       </c>
       <c r="M75" s="28" t="s">
         <v>5</v>
@@ -6776,7 +6786,7 @@
         <v>5</v>
       </c>
       <c r="O75" s="58" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="P75" s="40" t="s">
         <v>51</v>
@@ -6793,7 +6803,7 @@
       <c r="T75" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="U75" s="65" t="s">
+      <c r="U75" s="36" t="s">
         <v>51</v>
       </c>
       <c r="V75" s="36" t="s">
@@ -6810,11 +6820,11 @@
       <c r="A76" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B76" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>75</v>
+      <c r="B76" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="D76" s="40" t="s">
         <v>51</v>
@@ -6831,7 +6841,7 @@
       <c r="H76" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="I76" s="58" t="s">
+      <c r="I76" s="27" t="s">
         <v>51</v>
       </c>
       <c r="J76" s="36" t="s">
@@ -6841,7 +6851,7 @@
         <v>5</v>
       </c>
       <c r="L76" s="36" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="M76" s="28" t="s">
         <v>5</v>
@@ -6849,7 +6859,7 @@
       <c r="N76" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="O76" s="58" t="s">
+      <c r="O76" s="53" t="s">
         <v>51</v>
       </c>
       <c r="P76" s="40" t="s">
@@ -6867,7 +6877,7 @@
       <c r="T76" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="U76" s="65" t="s">
+      <c r="U76" s="36" t="s">
         <v>51</v>
       </c>
       <c r="V76" s="36" t="s">
@@ -6888,7 +6898,7 @@
         <v>73</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D77" s="40" t="s">
         <v>51</v>
@@ -6915,7 +6925,7 @@
         <v>5</v>
       </c>
       <c r="L77" s="36" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
       <c r="M77" s="28" t="s">
         <v>5</v>
@@ -6941,7 +6951,7 @@
       <c r="T77" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="U77" s="36" t="s">
+      <c r="U77" s="65" t="s">
         <v>51</v>
       </c>
       <c r="V77" s="36" t="s">
@@ -6954,15 +6964,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:24" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="41" t="s">
+    <row r="78" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B78" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>78</v>
+      <c r="B78" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="D78" s="40" t="s">
         <v>51</v>
@@ -6979,17 +6989,17 @@
       <c r="H78" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="I78" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="J78" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="K78" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="L78" s="27" t="s">
-        <v>51</v>
+      <c r="I78" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="J78" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K78" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L78" s="36" t="s">
+        <v>75</v>
       </c>
       <c r="M78" s="28" t="s">
         <v>5</v>
@@ -6997,46 +7007,46 @@
       <c r="N78" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="O78" s="27" t="s">
+      <c r="O78" s="58" t="s">
         <v>51</v>
       </c>
       <c r="P78" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="Q78" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="R78" s="40" t="s">
+      <c r="Q78" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="R78" s="41" t="s">
         <v>51</v>
       </c>
       <c r="S78" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="T78" s="40" t="s">
+      <c r="T78" s="19" t="s">
         <v>51</v>
       </c>
       <c r="U78" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="V78" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="W78" s="40" t="s">
+      <c r="V78" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="W78" s="41" t="s">
         <v>51</v>
       </c>
       <c r="X78" s="41" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>79</v>
+      <c r="B79" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="D79" s="40" t="s">
         <v>51</v>
@@ -7048,13 +7058,13 @@
         <v>51</v>
       </c>
       <c r="G79" s="40" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="H79" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="I79" s="27" t="s">
-        <v>74</v>
+      <c r="I79" s="58" t="s">
+        <v>51</v>
       </c>
       <c r="J79" s="36" t="s">
         <v>51</v>
@@ -7063,7 +7073,7 @@
         <v>5</v>
       </c>
       <c r="L79" s="36" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="M79" s="28" t="s">
         <v>5</v>
@@ -7071,20 +7081,20 @@
       <c r="N79" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="O79" s="27" t="s">
-        <v>74</v>
+      <c r="O79" s="58" t="s">
+        <v>51</v>
       </c>
       <c r="P79" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q79" s="40" t="s">
-        <v>74</v>
+        <v>51</v>
+      </c>
+      <c r="Q79" s="41" t="s">
+        <v>51</v>
       </c>
       <c r="R79" s="41" t="s">
         <v>51</v>
       </c>
       <c r="S79" s="40" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="T79" s="19" t="s">
         <v>51</v>
@@ -7102,15 +7112,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
+    <row r="80" spans="1:24" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="41" t="s">
         <v>43</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>77</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D80" s="40" t="s">
         <v>51</v>
@@ -7122,58 +7132,58 @@
         <v>51</v>
       </c>
       <c r="G80" s="40" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="H80" s="40" t="s">
         <v>51</v>
       </c>
       <c r="I80" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="J80" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="K80" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="L80" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="M80" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N80" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="O80" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="P80" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q80" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="R80" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="S80" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="T80" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="U80" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="V80" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="W80" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="X80" s="41" t="s">
         <v>75</v>
-      </c>
-      <c r="J80" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="K80" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L80" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M80" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="N80" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="O80" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="P80" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q80" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="R80" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="S80" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="T80" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="U80" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="V80" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="W80" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="X80" s="41" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="81" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -7184,7 +7194,7 @@
         <v>77</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D81" s="40" t="s">
         <v>51</v>
@@ -7196,45 +7206,45 @@
         <v>51</v>
       </c>
       <c r="G81" s="40" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="H81" s="40" t="s">
         <v>51</v>
       </c>
       <c r="I81" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="J81" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K81" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L81" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="M81" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N81" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="O81" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="P81" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="J81" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="K81" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L81" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M81" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="N81" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="O81" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="P81" s="40" t="s">
-        <v>51</v>
-      </c>
       <c r="Q81" s="40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R81" s="41" t="s">
         <v>51</v>
       </c>
       <c r="S81" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="T81" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="T81" s="19" t="s">
         <v>51</v>
       </c>
       <c r="U81" s="36" t="s">
@@ -7258,7 +7268,7 @@
         <v>77</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D82" s="40" t="s">
         <v>51</v>
@@ -7269,14 +7279,14 @@
       <c r="F82" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="G82" s="56" t="s">
+      <c r="G82" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="H82" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="I82" s="27" t="s">
         <v>75</v>
-      </c>
-      <c r="H82" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="I82" s="27" t="s">
-        <v>132</v>
       </c>
       <c r="J82" s="36" t="s">
         <v>51</v>
@@ -7300,16 +7310,16 @@
         <v>51</v>
       </c>
       <c r="Q82" s="40" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="R82" s="41" t="s">
         <v>51</v>
       </c>
       <c r="S82" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="T82" s="40" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="T82" s="56" t="s">
+        <v>51</v>
       </c>
       <c r="U82" s="36" t="s">
         <v>51</v>
@@ -7332,98 +7342,236 @@
         <v>77</v>
       </c>
       <c r="C83" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D83" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E83" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F83" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G83" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H83" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="I83" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="J83" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K83" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L83" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="M83" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N83" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="O83" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="P83" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q83" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="R83" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="S83" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="T83" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="U83" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="V83" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="W83" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="X83" s="41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D84" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E84" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F84" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G84" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="H84" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="I84" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="J84" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K84" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L84" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="M84" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N84" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="O84" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="P84" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q84" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="R84" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="S84" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="T84" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="U84" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="V84" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="W84" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="X84" s="41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C85" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D83" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E83" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F83" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="G83" s="56" t="s">
+      <c r="D85" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E85" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F85" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G85" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="H83" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="I83" s="27" t="s">
+      <c r="H85" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="I85" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="J83" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="K83" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L83" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M83" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="N83" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="O83" s="27" t="s">
+      <c r="J85" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K85" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L85" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="M85" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N85" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="O85" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="P83" s="40" t="s">
+      <c r="P85" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="Q83" s="40" t="s">
+      <c r="Q85" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="R83" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="S83" s="40" t="s">
+      <c r="R85" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="S85" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="T83" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="U83" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="V83" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="W83" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="X83" s="41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D84" s="40"/>
-      <c r="E84" s="40"/>
-      <c r="F84" s="40"/>
-      <c r="P84" s="40"/>
-    </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E85" s="40"/>
-      <c r="F85" s="40"/>
-      <c r="H85" s="36"/>
-      <c r="P85" s="40"/>
+      <c r="T85" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="U85" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="V85" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="W85" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="X85" s="41" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D86" s="40"/>
       <c r="E86" s="40"/>
       <c r="F86" s="40"/>
-      <c r="H86" s="36"/>
       <c r="P86" s="40"/>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E87" s="40"/>
       <c r="F87" s="40"/>
+      <c r="H87" s="36"/>
       <c r="P87" s="40"/>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E88" s="40"/>
       <c r="F88" s="40"/>
+      <c r="H88" s="36"/>
       <c r="P88" s="40"/>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
@@ -10618,9 +10766,13 @@
     </row>
     <row r="727" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E727" s="40"/>
+      <c r="F727" s="40"/>
+      <c r="P727" s="40"/>
     </row>
     <row r="728" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E728" s="40"/>
+      <c r="F728" s="40"/>
+      <c r="P728" s="40"/>
     </row>
     <row r="729" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E729" s="40"/>
@@ -19624,6 +19776,12 @@
     </row>
     <row r="3729" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E3729" s="40"/>
+    </row>
+    <row r="3730" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E3730" s="40"/>
+    </row>
+    <row r="3731" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E3731" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19640,11 +19798,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20125,8 +20283,8 @@
       <c r="F7" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="G7" s="40" t="s">
-        <v>75</v>
+      <c r="G7" s="71" t="s">
+        <v>74</v>
       </c>
       <c r="H7" s="27" t="s">
         <v>74</v>
@@ -20200,8 +20358,8 @@
       <c r="F8" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="G8" s="40" t="s">
-        <v>75</v>
+      <c r="G8" s="71" t="s">
+        <v>74</v>
       </c>
       <c r="H8" s="27" t="s">
         <v>74</v>
@@ -21063,8 +21221,8 @@
       <c r="S19" s="20">
         <v>1</v>
       </c>
-      <c r="T19" s="20">
-        <v>0</v>
+      <c r="T19" s="72">
+        <v>1</v>
       </c>
       <c r="U19" s="16">
         <v>1</v>
@@ -21547,8 +21705,8 @@
       <c r="F26" s="20">
         <v>1</v>
       </c>
-      <c r="G26" s="20">
-        <v>1</v>
+      <c r="G26" s="72">
+        <v>0</v>
       </c>
       <c r="H26" s="16">
         <v>1</v>
@@ -21559,8 +21717,8 @@
       <c r="J26" s="20">
         <v>0</v>
       </c>
-      <c r="K26" s="20">
-        <v>1</v>
+      <c r="K26" s="72">
+        <v>0</v>
       </c>
       <c r="L26" s="16">
         <v>1</v>
@@ -21633,8 +21791,8 @@
       <c r="J27" s="20">
         <v>1</v>
       </c>
-      <c r="K27" s="20">
-        <v>1</v>
+      <c r="K27" s="72">
+        <v>0</v>
       </c>
       <c r="L27" s="16">
         <v>1</v>
@@ -21707,8 +21865,8 @@
       <c r="J28" s="20">
         <v>1</v>
       </c>
-      <c r="K28" s="20">
-        <v>1</v>
+      <c r="K28" s="72">
+        <v>0</v>
       </c>
       <c r="L28" s="16">
         <v>1</v>

</xml_diff>

<commit_message>
feeding larvae hyphen fix dammit
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="740" windowWidth="21740" windowHeight="16640"/>
+    <workbookView xWindow="7580" yWindow="900" windowWidth="21740" windowHeight="16640"/>
   </bookViews>
   <sheets>
     <sheet name="sensitivity" sheetId="1" r:id="rId1"/>
@@ -698,22 +698,22 @@
     <t xml:space="preserve">no </t>
   </si>
   <si>
-    <t>feeding -calcifier</t>
-  </si>
-  <si>
-    <t>feeding - non-calcifier</t>
-  </si>
-  <si>
-    <t>non-feeding - calcifier</t>
-  </si>
-  <si>
-    <t>non-feeding - non-calcifier</t>
-  </si>
-  <si>
     <t>no larva</t>
   </si>
   <si>
     <t>habitat forming</t>
+  </si>
+  <si>
+    <t>feeding calcifier</t>
+  </si>
+  <si>
+    <t>feeding non-calcifier</t>
+  </si>
+  <si>
+    <t>non-feeding calcifier</t>
+  </si>
+  <si>
+    <t>non-feeding non-calcifier</t>
   </si>
 </sst>
 </file>
@@ -1044,11 +1044,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sens_traits" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1340,7 +1340,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1350,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB3731"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1456,7 +1456,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>5</v>
@@ -1530,7 +1530,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>5</v>
@@ -1604,7 +1604,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>5</v>
@@ -1678,7 +1678,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D5" s="36" t="s">
         <v>5</v>
@@ -1752,7 +1752,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>5</v>
@@ -3861,7 +3861,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="73" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C36" s="73" t="s">
         <v>15</v>
@@ -3935,7 +3935,7 @@
         <v>32</v>
       </c>
       <c r="B37" s="73" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C37" s="73" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
added exposure modifier for sst rise spec ad cap
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohara/github/spp_vuln_framework/_raw_data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFDDB0F-05F0-774A-B2D4-99C23C3F4F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A2810B-F020-C54C-A24B-3C04A1707E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="2680" windowWidth="25240" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4060" yWindow="2680" windowWidth="25240" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensitivity" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2986" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="226">
   <si>
     <t>category</t>
   </si>
@@ -777,7 +777,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -847,12 +847,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="21">
@@ -1185,7 +1179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1237,7 +1231,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1457,7 +1451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD3731"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -20497,11 +20491,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y2" sqref="Y2"/>
+      <selection pane="bottomRight" activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22043,8 +22037,8 @@
       <c r="W19" s="16">
         <v>1</v>
       </c>
-      <c r="X19" s="53" t="s">
-        <v>44</v>
+      <c r="X19" s="53">
+        <v>1</v>
       </c>
       <c r="Y19" s="16">
         <v>0</v>
@@ -22123,8 +22117,8 @@
       <c r="W20" s="16">
         <v>1</v>
       </c>
-      <c r="X20" s="53" t="s">
-        <v>44</v>
+      <c r="X20" s="53">
+        <v>1</v>
       </c>
       <c r="Y20" s="20">
         <v>1</v>
@@ -22204,8 +22198,8 @@
       <c r="W21" s="16">
         <v>0</v>
       </c>
-      <c r="X21" s="53" t="s">
-        <v>44</v>
+      <c r="X21" s="53">
+        <v>0</v>
       </c>
       <c r="Y21" s="20">
         <v>1</v>
@@ -22285,8 +22279,8 @@
       <c r="W22" s="16">
         <v>0</v>
       </c>
-      <c r="X22" s="53" t="s">
-        <v>44</v>
+      <c r="X22" s="53">
+        <v>0</v>
       </c>
       <c r="Y22" s="20">
         <v>0</v>
@@ -22366,8 +22360,8 @@
       <c r="W23" s="16">
         <v>0</v>
       </c>
-      <c r="X23" s="53" t="s">
-        <v>44</v>
+      <c r="X23" s="53">
+        <v>0</v>
       </c>
       <c r="Y23" s="20">
         <v>0</v>
@@ -22447,8 +22441,8 @@
       <c r="W24" s="16">
         <v>0</v>
       </c>
-      <c r="X24" s="53" t="s">
-        <v>44</v>
+      <c r="X24" s="53">
+        <v>0</v>
       </c>
       <c r="Y24" s="20">
         <v>0</v>
@@ -22528,8 +22522,8 @@
       <c r="W25" s="16">
         <v>1</v>
       </c>
-      <c r="X25" s="53" t="s">
-        <v>44</v>
+      <c r="X25" s="53">
+        <v>1</v>
       </c>
       <c r="Y25" s="20">
         <v>1</v>
@@ -22608,8 +22602,8 @@
       <c r="W26" s="16">
         <v>1</v>
       </c>
-      <c r="X26" s="53" t="s">
-        <v>44</v>
+      <c r="X26" s="53">
+        <v>1</v>
       </c>
       <c r="Y26" s="20">
         <v>1</v>
@@ -22688,8 +22682,8 @@
       <c r="W27" s="16">
         <v>1</v>
       </c>
-      <c r="X27" s="53" t="s">
-        <v>44</v>
+      <c r="X27" s="53">
+        <v>0</v>
       </c>
       <c r="Y27" s="20">
         <v>1</v>
@@ -22768,8 +22762,8 @@
       <c r="W28" s="16">
         <v>0</v>
       </c>
-      <c r="X28" s="53" t="s">
-        <v>44</v>
+      <c r="X28" s="53">
+        <v>0</v>
       </c>
       <c r="Y28" s="20">
         <v>1</v>
@@ -22848,8 +22842,8 @@
       <c r="W29" s="16">
         <v>0</v>
       </c>
-      <c r="X29" s="53" t="s">
-        <v>44</v>
+      <c r="X29" s="53">
+        <v>0</v>
       </c>
       <c r="Y29" s="20">
         <v>1</v>

</xml_diff>

<commit_message>
ugh forgot to make a row for the sst rise sensitivity trait
Former-commit-id: 39e12e7d00c37f8823141e469089ca2f2609dc41
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohara/github/spp_vuln_framework/_raw_data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A2810B-F020-C54C-A24B-3C04A1707E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF1D330-0825-9945-B869-70C3565E0FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="2680" windowWidth="25240" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4060" yWindow="2680" windowWidth="25240" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensitivity" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3001" uniqueCount="226">
   <si>
     <t>category</t>
   </si>
@@ -737,12 +737,6 @@
     <t>biomass removal</t>
   </si>
   <si>
-    <t>biomass removal vulnerability trait</t>
-  </si>
-  <si>
-    <t>vulnerable</t>
-  </si>
-  <si>
     <t>not larvae</t>
   </si>
   <si>
@@ -771,6 +765,12 @@
   </si>
   <si>
     <t>sst_rise</t>
+  </si>
+  <si>
+    <t>biomass removal sensitivity trait</t>
+  </si>
+  <si>
+    <t>sst rise sensitivity trait</t>
   </si>
 </sst>
 </file>
@@ -1451,11 +1451,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD3731"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y1" sqref="Y1"/>
+      <selection pane="bottomRight" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1549,10 +1549,10 @@
         <v>108</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="Y1" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Z1" s="15" t="s">
         <v>116</v>
@@ -2045,10 +2045,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="75" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D8" s="41" t="s">
         <v>67</v>
@@ -2125,10 +2125,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="75" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>219</v>
       </c>
       <c r="D9" s="41" t="s">
         <v>67</v>
@@ -2205,10 +2205,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="75" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D10" s="41" t="s">
         <v>68</v>
@@ -2285,10 +2285,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D11" s="41" t="s">
         <v>68</v>
@@ -2365,10 +2365,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="75" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D12" s="41" t="s">
         <v>124</v>
@@ -2445,10 +2445,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="75" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D13" s="41" t="s">
         <v>124</v>
@@ -8172,92 +8172,167 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:27" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="9" t="s">
+    <row r="86" spans="1:27" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B86" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E86" s="9" t="s">
+      <c r="B86" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="J86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="K86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="M86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="N86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="P86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="R86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="S86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="T86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="U86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="V86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="W86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="X86" s="74" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z86" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA86" s="9"/>
-    </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="F87" s="40"/>
-      <c r="G87" s="40"/>
-      <c r="I87" s="36"/>
-      <c r="Q87" s="40"/>
+      <c r="F86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="U86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X86" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA86" s="5"/>
+    </row>
+    <row r="87" spans="1:27" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="U87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X87" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA87" s="5"/>
     </row>
     <row r="88" spans="1:27" x14ac:dyDescent="0.2">
       <c r="F88" s="40"/>
@@ -20491,7 +20566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -20580,10 +20655,10 @@
         <v>108</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="Y1" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Z1" s="15" t="s">
         <v>116</v>
@@ -21732,7 +21807,7 @@
         <v>87</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D16" s="47" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
unchecked mesopelagic exposure to marine heat waves - literature seems to indicate the bulk of impacts are in the surface layers, down to 150 m, maybe a little deeper.
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casey\Documents\github\spp_vuln_framework\_raw_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAC02FC-A8A9-4AE1-91BD-A6EEC54E863D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654A122E-AC82-4208-B512-3A4350BAABF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="25290" windowHeight="13200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensitivity" sheetId="1" r:id="rId1"/>
@@ -20567,10 +20567,10 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="P5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomRight" activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -22277,7 +22277,7 @@
         <v>0</v>
       </c>
       <c r="Y21" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="16">
         <v>0</v>

</xml_diff>

<commit_message>
changing sensitivity from internal calcium structure to "low"
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casey\Documents\github\spp_vuln_framework\_raw_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50526033-405B-4F3A-8120-E8C3E12ADD45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3178AF-CDD2-48B4-81DD-73B1DEE39B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="25290" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1432,10 +1432,10 @@
   <dimension ref="A1:AD3731"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N69" sqref="N69"/>
+      <selection pane="bottomRight" activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5544,7 +5544,7 @@
         <v>44</v>
       </c>
       <c r="N53" s="12" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="O53" s="32" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
updated stressor scoring for UV and SLR
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casey\Documents\github\spp_vuln_framework\_raw_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3178AF-CDD2-48B4-81DD-73B1DEE39B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DC8144-2290-4612-B338-C8D8A29F98C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="25290" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,6 +37,11 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={84D5D8E3-339B-6E45-8600-A1BE013116C5}</author>
+    <author>tc={460808FA-53C5-4E91-A3CA-C4664C4A3D24}</author>
+    <author>tc={AE2FD34B-F026-46A4-A124-1055B6D24641}</author>
+    <author>tc={D34E475D-F200-4278-AC56-15CC6D59A8F4}</author>
+    <author>tc={B5D81856-018C-46A3-87BE-037B9A24C4A2}</author>
+    <author>tc={0D1001FB-99A0-471C-B2B4-A90AF69A7BDA}</author>
   </authors>
   <commentList>
     <comment ref="X1" authorId="0" shapeId="0" xr:uid="{84D5D8E3-339B-6E45-8600-A1BE013116C5}">
@@ -45,6 +50,46 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     this will manually be set to 1 for all species - high sensitivity if thermal max tolerance is exceeded</t>
+      </text>
+    </comment>
+    <comment ref="U29" authorId="1" shapeId="0" xr:uid="{460808FA-53C5-4E91-A3CA-C4664C4A3D24}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was "high" - but a few mm a year of SLR should not be sufficient to overcome photosynthesis - if this is to get at corals, it's not the photosynthesis that's problematic, but the rate of reef growth</t>
+      </text>
+    </comment>
+    <comment ref="W29" authorId="2" shapeId="0" xr:uid="{AE2FD34B-F026-46A4-A124-1055B6D24641}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Additive with effect of planktonic stages</t>
+      </text>
+    </comment>
+    <comment ref="U32" authorId="3" shapeId="0" xr:uid="{D34E475D-F200-4278-AC56-15CC6D59A8F4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was "high" - but not all surface critters care about SLR e.g. whales or whale sharks</t>
+      </text>
+    </comment>
+    <comment ref="U38" authorId="4" shapeId="0" xr:uid="{B5D81856-018C-46A3-87BE-037B9A24C4A2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was "high" - certainly SLR affects ocean-adjacent terrestrial habitats, but at slow rates</t>
+      </text>
+    </comment>
+    <comment ref="U73" authorId="5" shapeId="0" xr:uid="{0D1001FB-99A0-471C-B2B4-A90AF69A7BDA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was "low" - but will a couple mm of SLR per year diminish light sufficiently to be problematic?</t>
       </text>
     </comment>
   </commentList>
@@ -777,7 +822,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -847,6 +892,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="21">
@@ -1104,6 +1155,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Casey O'Hara" id="{DA942791-E096-4CC4-BAE2-5DA30CA09C57}" userId="4066c19ab0333d2e" providerId="Windows Live"/>
   <person displayName="Casey O'Hara" id="{2DA28BFC-C461-F94E-97AB-9309C9AABAE3}" userId="S::cohara@ucsb.edu::2eca58cb-2860-4e2f-adc1-5de11af13c09" providerId="AD"/>
 </personList>
 </file>
@@ -1416,6 +1468,21 @@
   <threadedComment ref="X1" dT="2022-01-15T21:59:52.98" personId="{2DA28BFC-C461-F94E-97AB-9309C9AABAE3}" id="{84D5D8E3-339B-6E45-8600-A1BE013116C5}">
     <text>this will manually be set to 1 for all species - high sensitivity if thermal max tolerance is exceeded</text>
   </threadedComment>
+  <threadedComment ref="U29" dT="2022-10-09T01:14:53.35" personId="{DA942791-E096-4CC4-BAE2-5DA30CA09C57}" id="{460808FA-53C5-4E91-A3CA-C4664C4A3D24}">
+    <text>Was "high" - but a few mm a year of SLR should not be sufficient to overcome photosynthesis - if this is to get at corals, it's not the photosynthesis that's problematic, but the rate of reef growth</text>
+  </threadedComment>
+  <threadedComment ref="W29" dT="2022-10-09T01:10:06.84" personId="{DA942791-E096-4CC4-BAE2-5DA30CA09C57}" id="{AE2FD34B-F026-46A4-A124-1055B6D24641}">
+    <text>Additive with effect of planktonic stages</text>
+  </threadedComment>
+  <threadedComment ref="U32" dT="2022-10-09T01:11:29.73" personId="{DA942791-E096-4CC4-BAE2-5DA30CA09C57}" id="{D34E475D-F200-4278-AC56-15CC6D59A8F4}">
+    <text>Was "high" - but not all surface critters care about SLR e.g. whales or whale sharks</text>
+  </threadedComment>
+  <threadedComment ref="U38" dT="2022-10-09T01:13:39.14" personId="{DA942791-E096-4CC4-BAE2-5DA30CA09C57}" id="{B5D81856-018C-46A3-87BE-037B9A24C4A2}">
+    <text>Was "high" - certainly SLR affects ocean-adjacent terrestrial habitats, but at slow rates</text>
+  </threadedComment>
+  <threadedComment ref="U73" dT="2022-10-09T01:12:31.16" personId="{DA942791-E096-4CC4-BAE2-5DA30CA09C57}" id="{0D1001FB-99A0-471C-B2B4-A90AF69A7BDA}">
+    <text>Was "low" - but will a couple mm of SLR per year diminish light sufficiently to be problematic?</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1432,10 +1499,10 @@
   <dimension ref="A1:AD3731"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N53" sqref="N53"/>
+      <selection pane="bottomRight" activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3755,13 +3822,13 @@
         <v>67</v>
       </c>
       <c r="U29" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="V29" t="s">
         <v>124</v>
       </c>
       <c r="W29" s="55" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="X29" s="58" t="s">
         <v>5</v>
@@ -3995,7 +4062,7 @@
         <v>44</v>
       </c>
       <c r="U32" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="V32" t="s">
         <v>124</v>
@@ -4365,7 +4432,7 @@
         <v>44</v>
       </c>
       <c r="U38" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
       <c r="V38" t="s">
         <v>124</v>
@@ -7165,7 +7232,7 @@
         <v>67</v>
       </c>
       <c r="U73" s="58" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="V73" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
updated stressor scores for SLR
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/stressors_traits_scored.xlsx
+++ b/_raw_data/xlsx/stressors_traits_scored.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casey\Documents\github\spp_vuln_framework\_raw_data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DC8144-2290-4612-B338-C8D8A29F98C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB4FE9E-D8F2-4254-B08A-A44CF2C2208F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="25290" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,11 +37,13 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={84D5D8E3-339B-6E45-8600-A1BE013116C5}</author>
+    <author>tc={A71617E6-9320-4946-AC2E-CFC24A35BB5C}</author>
     <author>tc={460808FA-53C5-4E91-A3CA-C4664C4A3D24}</author>
     <author>tc={AE2FD34B-F026-46A4-A124-1055B6D24641}</author>
     <author>tc={D34E475D-F200-4278-AC56-15CC6D59A8F4}</author>
     <author>tc={B5D81856-018C-46A3-87BE-037B9A24C4A2}</author>
     <author>tc={0D1001FB-99A0-471C-B2B4-A90AF69A7BDA}</author>
+    <author>tc={320BA74A-9014-4289-9971-C703E485599E}</author>
   </authors>
   <commentList>
     <comment ref="X1" authorId="0" shapeId="0" xr:uid="{84D5D8E3-339B-6E45-8600-A1BE013116C5}">
@@ -52,7 +54,15 @@
     this will manually be set to 1 for all species - high sensitivity if thermal max tolerance is exceeded</t>
       </text>
     </comment>
-    <comment ref="U29" authorId="1" shapeId="0" xr:uid="{460808FA-53C5-4E91-A3CA-C4664C4A3D24}">
+    <comment ref="U16" authorId="1" shapeId="0" xr:uid="{A71617E6-9320-4946-AC2E-CFC24A35BB5C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was "low" but SLR and salinity are distinct from one another…?</t>
+      </text>
+    </comment>
+    <comment ref="U29" authorId="2" shapeId="0" xr:uid="{460808FA-53C5-4E91-A3CA-C4664C4A3D24}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -60,7 +70,7 @@
     Was "high" - but a few mm a year of SLR should not be sufficient to overcome photosynthesis - if this is to get at corals, it's not the photosynthesis that's problematic, but the rate of reef growth</t>
       </text>
     </comment>
-    <comment ref="W29" authorId="2" shapeId="0" xr:uid="{AE2FD34B-F026-46A4-A124-1055B6D24641}">
+    <comment ref="W29" authorId="3" shapeId="0" xr:uid="{AE2FD34B-F026-46A4-A124-1055B6D24641}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -68,7 +78,7 @@
     Additive with effect of planktonic stages</t>
       </text>
     </comment>
-    <comment ref="U32" authorId="3" shapeId="0" xr:uid="{D34E475D-F200-4278-AC56-15CC6D59A8F4}">
+    <comment ref="U32" authorId="4" shapeId="0" xr:uid="{D34E475D-F200-4278-AC56-15CC6D59A8F4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -76,7 +86,7 @@
     Was "high" - but not all surface critters care about SLR e.g. whales or whale sharks</t>
       </text>
     </comment>
-    <comment ref="U38" authorId="4" shapeId="0" xr:uid="{B5D81856-018C-46A3-87BE-037B9A24C4A2}">
+    <comment ref="U38" authorId="5" shapeId="0" xr:uid="{B5D81856-018C-46A3-87BE-037B9A24C4A2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -84,12 +94,20 @@
     Was "high" - certainly SLR affects ocean-adjacent terrestrial habitats, but at slow rates</t>
       </text>
     </comment>
-    <comment ref="U73" authorId="5" shapeId="0" xr:uid="{0D1001FB-99A0-471C-B2B4-A90AF69A7BDA}">
+    <comment ref="U73" authorId="6" shapeId="0" xr:uid="{0D1001FB-99A0-471C-B2B4-A90AF69A7BDA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Was "low" - but will a couple mm of SLR per year diminish light sufficiently to be problematic?</t>
+      </text>
+    </comment>
+    <comment ref="U84" authorId="7" shapeId="0" xr:uid="{320BA74A-9014-4289-9971-C703E485599E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Was "high" - but no mangroves anymore, so drop this to avoid confusion</t>
       </text>
     </comment>
   </commentList>
@@ -1468,6 +1486,9 @@
   <threadedComment ref="X1" dT="2022-01-15T21:59:52.98" personId="{2DA28BFC-C461-F94E-97AB-9309C9AABAE3}" id="{84D5D8E3-339B-6E45-8600-A1BE013116C5}">
     <text>this will manually be set to 1 for all species - high sensitivity if thermal max tolerance is exceeded</text>
   </threadedComment>
+  <threadedComment ref="U16" dT="2022-10-09T20:56:22.79" personId="{DA942791-E096-4CC4-BAE2-5DA30CA09C57}" id="{A71617E6-9320-4946-AC2E-CFC24A35BB5C}">
+    <text>Was "low" but SLR and salinity are distinct from one another…?</text>
+  </threadedComment>
   <threadedComment ref="U29" dT="2022-10-09T01:14:53.35" personId="{DA942791-E096-4CC4-BAE2-5DA30CA09C57}" id="{460808FA-53C5-4E91-A3CA-C4664C4A3D24}">
     <text>Was "high" - but a few mm a year of SLR should not be sufficient to overcome photosynthesis - if this is to get at corals, it's not the photosynthesis that's problematic, but the rate of reef growth</text>
   </threadedComment>
@@ -1482,6 +1503,9 @@
   </threadedComment>
   <threadedComment ref="U73" dT="2022-10-09T01:12:31.16" personId="{DA942791-E096-4CC4-BAE2-5DA30CA09C57}" id="{0D1001FB-99A0-471C-B2B4-A90AF69A7BDA}">
     <text>Was "low" - but will a couple mm of SLR per year diminish light sufficiently to be problematic?</text>
+  </threadedComment>
+  <threadedComment ref="U84" dT="2022-10-09T20:55:29.51" personId="{DA942791-E096-4CC4-BAE2-5DA30CA09C57}" id="{320BA74A-9014-4289-9971-C703E485599E}">
+    <text>Was "high" - but no mangroves anymore, so drop this to avoid confusion</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1499,10 +1523,10 @@
   <dimension ref="A1:AD3731"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U30" sqref="U30"/>
+      <selection pane="bottomRight" activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2782,7 +2806,7 @@
         <v>44</v>
       </c>
       <c r="U16" s="58" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="V16" t="s">
         <v>124</v>
@@ -8112,7 +8136,7 @@
         <v>44</v>
       </c>
       <c r="U84" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="V84" t="s">
         <v>44</v>

</xml_diff>